<commit_message>
added sim data files again
</commit_message>
<xml_diff>
--- a/cal/cal_results/CS_Ilena_Scattering_Results.xlsx
+++ b/cal/cal_results/CS_Ilena_Scattering_Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonny Woof\Google Drive\Python_packages_woof\pyMAP\cal\cal_results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92D9AA89-2660-46D0-AE77-DC92B1EB1129}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA0BD6EF-317D-41BF-9BF4-5A3AA53654E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-11550" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cutfit fwhm" sheetId="3" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="63">
   <si>
     <t>100A</t>
   </si>
@@ -217,6 +217,12 @@
   </si>
   <si>
     <t>xxx</t>
+  </si>
+  <si>
+    <t>e_loss</t>
+  </si>
+  <si>
+    <t>None</t>
   </si>
 </sst>
 </file>
@@ -546,7 +552,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -606,6 +612,14 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -886,10 +900,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:AL209"/>
+  <dimension ref="A2:AS209"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A145" zoomScale="77" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="Q183" sqref="Q183"/>
+    <sheetView tabSelected="1" topLeftCell="F159" zoomScale="77" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="R187" sqref="R187"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -899,17 +913,18 @@
     <col min="9" max="9" width="11.5546875" style="13"/>
     <col min="15" max="15" width="11.5546875" style="13"/>
     <col min="20" max="20" width="11.5546875" style="14"/>
-    <col min="21" max="21" width="24.88671875" customWidth="1"/>
+    <col min="21" max="27" width="11.5546875" style="49"/>
+    <col min="28" max="28" width="24.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="AA2" s="44" t="s">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="AH2" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="AB2" s="45"/>
-      <c r="AC2" s="46"/>
-    </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="AI2" s="45"/>
+      <c r="AJ2" s="46"/>
+    </row>
+    <row r="3" spans="1:36" x14ac:dyDescent="0.3">
       <c r="I3" s="13" t="s">
         <v>10</v>
       </c>
@@ -922,28 +937,28 @@
       <c r="Q3" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="W3" s="47" t="s">
+      <c r="AD3" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="X3" s="48"/>
-      <c r="AA3" s="3" t="s">
+      <c r="AE3" s="48"/>
+      <c r="AH3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="AB3" t="s">
+      <c r="AI3" t="s">
         <v>15</v>
       </c>
-      <c r="AC3" s="4" t="s">
+      <c r="AJ3" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:36" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="I4" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="AA4" s="3"/>
-      <c r="AC4" s="4"/>
-    </row>
-    <row r="5" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AH4" s="3"/>
+      <c r="AJ4" s="4"/>
+    </row>
+    <row r="5" spans="1:36" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="I5" s="13" t="s">
         <v>10</v>
       </c>
@@ -980,28 +995,49 @@
       <c r="T5" t="s">
         <v>38</v>
       </c>
-      <c r="V5" s="2"/>
-      <c r="W5" s="12" t="s">
+      <c r="U5" t="s">
+        <v>62</v>
+      </c>
+      <c r="V5" t="s">
+        <v>62</v>
+      </c>
+      <c r="W5" t="s">
+        <v>62</v>
+      </c>
+      <c r="X5" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>62</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>62</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>62</v>
+      </c>
+      <c r="AC5" s="2"/>
+      <c r="AD5" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="X5" s="2"/>
-      <c r="Y5" s="2"/>
-      <c r="Z5" t="s">
+      <c r="AE5" s="2"/>
+      <c r="AF5" s="2"/>
+      <c r="AG5" t="s">
         <v>27</v>
       </c>
-      <c r="AA5" s="5">
+      <c r="AH5" s="5">
         <v>0.5</v>
       </c>
-      <c r="AB5">
+      <c r="AI5">
         <f>2*SQRT(2*LN(2))</f>
         <v>2.3548200450309493</v>
       </c>
-      <c r="AC5" s="4">
-        <f>AB5/AB5</f>
+      <c r="AJ5" s="4">
+        <f>AI5/AI5</f>
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:36" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>40</v>
       </c>
@@ -1068,22 +1104,43 @@
         <f t="shared" si="0"/>
         <v>1000</v>
       </c>
-      <c r="W6" s="10" t="s">
+      <c r="U6" s="49">
+        <v>14</v>
+      </c>
+      <c r="V6" s="49">
+        <v>27</v>
+      </c>
+      <c r="W6" s="49">
+        <v>52</v>
+      </c>
+      <c r="X6" s="56">
+        <v>102</v>
+      </c>
+      <c r="Y6" s="56">
+        <v>197</v>
+      </c>
+      <c r="Z6" s="56">
+        <v>451</v>
+      </c>
+      <c r="AA6" s="56">
+        <v>908</v>
+      </c>
+      <c r="AD6" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="AA6" s="5">
+      <c r="AH6" s="5">
         <v>0.6</v>
       </c>
-      <c r="AB6">
+      <c r="AI6">
         <f>2*SQRT(2*(-LN(3)+LN(5)))</f>
         <v>2.021535305189579</v>
       </c>
-      <c r="AC6" s="6">
-        <f>AB6/AB$5</f>
+      <c r="AJ6" s="6">
+        <f>AI6/AI$5</f>
         <v>0.85846700237470164</v>
       </c>
     </row>
-    <row r="7" spans="1:29" s="30" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:36" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="29" t="s">
         <v>41</v>
       </c>
@@ -1150,19 +1207,19 @@
         <f>10+10.5</f>
         <v>20.5</v>
       </c>
-      <c r="AA7" s="35">
+      <c r="AH7" s="35">
         <v>0.7</v>
       </c>
-      <c r="AB7" s="30">
+      <c r="AI7" s="30">
         <f>2* SQRT(2* (LN(2) + LN(5) - LN(7)))</f>
         <v>1.6892008618011825</v>
       </c>
-      <c r="AC7" s="36">
-        <f t="shared" ref="AC7:AC9" si="1">AB7/AB$5</f>
+      <c r="AJ7" s="36">
+        <f t="shared" ref="AJ7:AJ9" si="1">AI7/AI$5</f>
         <v>0.71733755849652681</v>
       </c>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A8" s="13"/>
       <c r="F8">
         <v>8</v>
@@ -1215,19 +1272,19 @@
         <f>16.1-2.8</f>
         <v>13.3</v>
       </c>
-      <c r="AA8" s="5">
+      <c r="AH8" s="5">
         <v>0.8</v>
       </c>
-      <c r="AB8">
+      <c r="AI8">
         <f>2* SQRT(2* (-2* LN(2) + LN(5)))</f>
         <v>1.3360944616731549</v>
       </c>
-      <c r="AC8" s="6">
+      <c r="AJ8" s="6">
         <f t="shared" si="1"/>
         <v>0.56738707677154787</v>
       </c>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A9" s="13"/>
       <c r="F9">
         <v>8</v>
@@ -1237,22 +1294,22 @@
       <c r="I9" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="V9" s="2">
+      <c r="AC9" s="2">
         <v>0.6</v>
       </c>
-      <c r="AA9" s="7">
+      <c r="AH9" s="7">
         <v>0.9</v>
       </c>
-      <c r="AB9" s="1">
+      <c r="AI9" s="1">
         <f>2* SQRT(2* (LN(2) - 2*LN(3) +LN(5)))</f>
         <v>0.91808721005284077</v>
       </c>
-      <c r="AC9" s="8">
+      <c r="AJ9" s="8">
         <f t="shared" si="1"/>
         <v>0.38987574103174172</v>
       </c>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A10" s="13"/>
       <c r="F10">
         <v>8</v>
@@ -1302,20 +1359,27 @@
       <c r="T10" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="V10">
+      <c r="U10" s="50"/>
+      <c r="V10" s="50"/>
+      <c r="W10" s="50"/>
+      <c r="X10" s="50"/>
+      <c r="Y10" s="50"/>
+      <c r="Z10" s="50"/>
+      <c r="AA10" s="50"/>
+      <c r="AC10">
         <f>10+8.5</f>
         <v>18.5</v>
       </c>
-      <c r="W10">
+      <c r="AD10">
         <f>10.5+9</f>
         <v>19.5</v>
       </c>
-      <c r="X10">
+      <c r="AE10">
         <f>10.6+9.1</f>
         <v>19.7</v>
       </c>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A11" s="13"/>
       <c r="F11">
         <v>8</v>
@@ -1368,23 +1432,23 @@
         <f>17-2.5</f>
         <v>14.5</v>
       </c>
-      <c r="V11" s="19">
-        <f>V10/AC6</f>
+      <c r="AC11" s="19">
+        <f>AC10/AJ6</f>
         <v>21.550042050335168</v>
       </c>
-      <c r="W11" s="19">
-        <f>W10/AC6</f>
+      <c r="AD11" s="19">
+        <f>AD10/AJ6</f>
         <v>22.714909188191122</v>
       </c>
-      <c r="X11" s="19">
-        <f>X10/AC6</f>
+      <c r="AE11" s="19">
+        <f>AE10/AJ6</f>
         <v>22.947882615762314</v>
       </c>
-      <c r="Y11" s="16" t="s">
+      <c r="AF11" s="16" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A12" s="13"/>
       <c r="F12">
         <v>8</v>
@@ -1394,7 +1458,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A13" s="13"/>
       <c r="F13">
         <v>8</v>
@@ -1448,7 +1512,7 @@
         <v>17.100000000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A14" s="13"/>
       <c r="F14">
         <v>8</v>
@@ -1502,7 +1566,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A15" s="13"/>
       <c r="F15">
         <v>8</v>
@@ -1511,14 +1575,14 @@
       <c r="I15" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="V15" s="2">
+      <c r="AC15" s="2">
         <v>0.6</v>
       </c>
-      <c r="W15" t="s">
+      <c r="AD15" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A16" s="13"/>
       <c r="F16">
         <v>8</v>
@@ -1570,16 +1634,23 @@
       <c r="T16" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="V16">
+      <c r="U16" s="50"/>
+      <c r="V16" s="50"/>
+      <c r="W16" s="50"/>
+      <c r="X16" s="50"/>
+      <c r="Y16" s="50"/>
+      <c r="Z16" s="50"/>
+      <c r="AA16" s="50"/>
+      <c r="AC16">
         <f>9+8.5</f>
         <v>17.5</v>
       </c>
-      <c r="W16" s="19">
-        <f>V16/AC6</f>
+      <c r="AD16" s="19">
+        <f>AC16/AJ6</f>
         <v>20.385174912479211</v>
       </c>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A17" s="13"/>
       <c r="F17">
         <v>8</v>
@@ -1633,21 +1704,21 @@
         <v>18.3</v>
       </c>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A18" s="13"/>
       <c r="F18">
         <v>8</v>
       </c>
       <c r="H18" s="11"/>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A19" s="13"/>
       <c r="F19">
         <v>8</v>
       </c>
       <c r="I19" s="15"/>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A20" s="13"/>
       <c r="E20">
         <v>2</v>
@@ -1693,7 +1764,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A21" s="13"/>
       <c r="F21">
         <v>8</v>
@@ -1736,21 +1807,21 @@
         <v>13.8</v>
       </c>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A22" s="13"/>
       <c r="F22">
         <v>8</v>
       </c>
       <c r="G22" s="11"/>
       <c r="H22" s="11"/>
-      <c r="V22" s="2" t="s">
+      <c r="AC22" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="Y22" s="2">
+      <c r="AF22" s="2">
         <v>0.7</v>
       </c>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A23" s="13"/>
       <c r="F23">
         <v>8</v>
@@ -1785,24 +1856,24 @@
       <c r="T23" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="V23">
+      <c r="AC23">
         <f>8.7+10.3</f>
         <v>19</v>
       </c>
-      <c r="W23">
+      <c r="AD23">
         <f>10.5+8.8</f>
         <v>19.3</v>
       </c>
-      <c r="X23">
+      <c r="AE23">
         <f>10.5+8.8</f>
         <v>19.3</v>
       </c>
-      <c r="Y23">
+      <c r="AF23">
         <f>9.3+7.2</f>
         <v>16.5</v>
       </c>
     </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A24" s="13"/>
       <c r="F24">
         <v>8</v>
@@ -1841,31 +1912,31 @@
         <f>17-2.1</f>
         <v>14.9</v>
       </c>
-      <c r="V24" s="19">
-        <f>V23/AC6</f>
+      <c r="AC24" s="19">
+        <f>AC23/AJ6</f>
         <v>22.132475619263143</v>
       </c>
-      <c r="W24" s="19">
-        <f>W23/AC6</f>
+      <c r="AD24" s="19">
+        <f>AD23/AJ6</f>
         <v>22.481935760619933</v>
       </c>
-      <c r="X24" s="19">
-        <f>X23/AC6</f>
+      <c r="AE24" s="19">
+        <f>AE23/AJ6</f>
         <v>22.481935760619933</v>
       </c>
-      <c r="Y24" s="19">
-        <f>Y23/AC7</f>
+      <c r="AF24" s="19">
+        <f>AF23/AJ7</f>
         <v>23.001723253669407</v>
       </c>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A25" s="13"/>
       <c r="F25">
         <v>8</v>
       </c>
       <c r="H25" s="11"/>
     </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A26" s="13"/>
       <c r="F26">
         <v>8</v>
@@ -1901,14 +1972,21 @@
         <v>17.2</v>
       </c>
       <c r="T26" s="18"/>
-      <c r="W26" t="s">
+      <c r="U26" s="50"/>
+      <c r="V26" s="50"/>
+      <c r="W26" s="50"/>
+      <c r="X26" s="50"/>
+      <c r="Y26" s="50"/>
+      <c r="Z26" s="50"/>
+      <c r="AA26" s="50"/>
+      <c r="AD26" t="s">
         <v>20</v>
       </c>
-      <c r="X26" t="s">
+      <c r="AE26" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A27" s="13"/>
       <c r="F27">
         <v>8</v>
@@ -1947,23 +2025,23 @@
         <f>17-2</f>
         <v>15</v>
       </c>
-      <c r="W27">
+      <c r="AD27">
         <f>9+7</f>
         <v>16</v>
       </c>
-      <c r="X27" s="19">
-        <f>W27/AC6</f>
+      <c r="AE27" s="19">
+        <f>AD27/AJ6</f>
         <v>18.63787420569528</v>
       </c>
     </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A28" s="13"/>
       <c r="F28">
         <v>8</v>
       </c>
       <c r="H28" s="11"/>
     </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A29" s="13"/>
       <c r="F29">
         <v>8</v>
@@ -2000,19 +2078,19 @@
       <c r="T29" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="V29" t="s">
+      <c r="AC29" t="s">
         <v>20</v>
       </c>
-      <c r="W29">
+      <c r="AD29">
         <f>9+8</f>
         <v>17</v>
       </c>
-      <c r="X29">
+      <c r="AE29">
         <f>9.4+8.6</f>
         <v>18</v>
       </c>
     </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A30" s="13"/>
       <c r="F30">
         <v>8</v>
@@ -2051,32 +2129,32 @@
         <f>19.9-1.9</f>
         <v>18</v>
       </c>
-      <c r="W30" s="19">
-        <f>W29/AC6</f>
+      <c r="AD30" s="19">
+        <f>AD29/AJ6</f>
         <v>19.802741343551233</v>
       </c>
-      <c r="X30" s="19">
-        <f>X29/AC6</f>
+      <c r="AE30" s="19">
+        <f>AE29/AJ6</f>
         <v>20.96760848140719</v>
       </c>
     </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A31" s="13"/>
       <c r="H31" s="11"/>
     </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A32" s="13"/>
       <c r="F32">
         <v>15</v>
       </c>
-      <c r="V32" s="2">
+      <c r="AC32" s="2">
         <v>0.7</v>
       </c>
-      <c r="Y32" s="2">
+      <c r="AF32" s="2">
         <v>0.8</v>
       </c>
     </row>
-    <row r="33" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A33" s="13"/>
       <c r="E33">
         <v>2</v>
@@ -2103,39 +2181,46 @@
         <v>25</v>
       </c>
       <c r="Q33" s="19">
-        <f>V33/$AC$7</f>
+        <f>AC33/$AJ$7</f>
         <v>23.001723253669407</v>
       </c>
       <c r="R33" s="19">
-        <f t="shared" ref="R33" si="2">W33/$AC$7</f>
+        <f t="shared" ref="R33" si="2">AD33/$AJ$7</f>
         <v>24.813980237291847</v>
       </c>
       <c r="S33" s="19">
-        <f t="shared" ref="S33" si="3">X33/$AC$7</f>
+        <f t="shared" ref="S33" si="3">AE33/$AJ$7</f>
         <v>27.183854754336572</v>
       </c>
       <c r="T33" s="20">
-        <f>Y33/$AC$8</f>
+        <f>AF33/$AJ$8</f>
         <v>27.494457732038136</v>
       </c>
-      <c r="V33">
+      <c r="U33" s="51"/>
+      <c r="V33" s="51"/>
+      <c r="W33" s="51"/>
+      <c r="X33" s="51"/>
+      <c r="Y33" s="51"/>
+      <c r="Z33" s="51"/>
+      <c r="AA33" s="51"/>
+      <c r="AC33">
         <f>9+7.5</f>
         <v>16.5</v>
       </c>
-      <c r="W33">
+      <c r="AD33">
         <f>9.3+8.5</f>
         <v>17.8</v>
       </c>
-      <c r="X33">
+      <c r="AE33">
         <f>9.5+10</f>
         <v>19.5</v>
       </c>
-      <c r="Y33">
+      <c r="AF33">
         <f>8.5+7.1</f>
         <v>15.6</v>
       </c>
     </row>
-    <row r="34" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A34" s="13"/>
       <c r="F34">
         <v>15</v>
@@ -2159,11 +2244,11 @@
         <v>22.08</v>
       </c>
       <c r="Q34" s="19">
-        <f>V34/$AC$7</f>
+        <f>AC34/$AJ$7</f>
         <v>19.098400519713387</v>
       </c>
       <c r="R34" s="19">
-        <f t="shared" ref="R34:S34" si="4">W34/$AC$7</f>
+        <f t="shared" ref="R34:S34" si="4">AD34/$AJ$7</f>
         <v>20.074231203202391</v>
       </c>
       <c r="S34" s="19">
@@ -2171,27 +2256,34 @@
         <v>22.304701336891547</v>
       </c>
       <c r="T34" s="20">
-        <f>Y34/$AC$8</f>
+        <f>AF34/$AJ$8</f>
         <v>21.502075918645211</v>
       </c>
-      <c r="V34">
+      <c r="U34" s="51"/>
+      <c r="V34" s="51"/>
+      <c r="W34" s="51"/>
+      <c r="X34" s="51"/>
+      <c r="Y34" s="51"/>
+      <c r="Z34" s="51"/>
+      <c r="AA34" s="51"/>
+      <c r="AC34">
         <f>19.5-5.8</f>
         <v>13.7</v>
       </c>
-      <c r="W34">
+      <c r="AD34">
         <f>19.7-5.3</f>
         <v>14.399999999999999</v>
       </c>
-      <c r="X34">
+      <c r="AE34">
         <f>21.2-5.2</f>
         <v>16</v>
       </c>
-      <c r="Y34">
+      <c r="AF34">
         <f>19.8-7.6</f>
         <v>12.200000000000001</v>
       </c>
     </row>
-    <row r="35" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A35" s="13"/>
       <c r="F35">
         <v>15</v>
@@ -2202,8 +2294,15 @@
       <c r="R35" s="21"/>
       <c r="S35" s="21"/>
       <c r="T35" s="22"/>
-    </row>
-    <row r="36" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="U35" s="52"/>
+      <c r="V35" s="52"/>
+      <c r="W35" s="52"/>
+      <c r="X35" s="52"/>
+      <c r="Y35" s="52"/>
+      <c r="Z35" s="52"/>
+      <c r="AA35" s="52"/>
+    </row>
+    <row r="36" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A36" s="13"/>
       <c r="F36">
         <v>15</v>
@@ -2227,11 +2326,11 @@
         <v>25</v>
       </c>
       <c r="Q36" s="19">
-        <f>V36/$AC$8</f>
+        <f>AC36/$AJ$8</f>
         <v>25.027006397111634</v>
       </c>
       <c r="R36" s="19">
-        <f t="shared" ref="R36:T36" si="5">W36/$AC$8</f>
+        <f t="shared" ref="R36:T36" si="5">AD36/$AJ$8</f>
         <v>25.203252921034959</v>
       </c>
       <c r="S36" s="19">
@@ -2242,27 +2341,34 @@
         <f t="shared" si="5"/>
         <v>28.551936875578065</v>
       </c>
-      <c r="V36">
+      <c r="U36" s="51"/>
+      <c r="V36" s="51"/>
+      <c r="W36" s="51"/>
+      <c r="X36" s="51"/>
+      <c r="Y36" s="51"/>
+      <c r="Z36" s="51"/>
+      <c r="AA36" s="51"/>
+      <c r="AC36">
         <f>7+7.2</f>
         <v>14.2</v>
       </c>
-      <c r="W36">
+      <c r="AD36">
         <f>7+7.3</f>
         <v>14.3</v>
       </c>
-      <c r="X36">
+      <c r="AE36">
         <f>7.5+7.7</f>
         <v>15.2</v>
       </c>
-      <c r="Y36">
+      <c r="AF36">
         <f>8+8.2</f>
         <v>16.2</v>
       </c>
-      <c r="Z36" t="s">
+      <c r="AG36" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="37" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A37" s="13"/>
       <c r="F37">
         <v>15</v>
@@ -2286,39 +2392,46 @@
         <v>21.3599999999999</v>
       </c>
       <c r="Q37" s="19">
-        <f>V37/$AC$8</f>
+        <f>AC37/$AJ$8</f>
         <v>21.502075918645208</v>
       </c>
       <c r="R37" s="19">
-        <f t="shared" ref="R37" si="6">W37/$AC$8</f>
+        <f t="shared" ref="R37" si="6">AD37/$AJ$8</f>
         <v>22.735801586108455</v>
       </c>
       <c r="S37" s="19">
-        <f t="shared" ref="S37" si="7">X37/$AC$8</f>
+        <f t="shared" ref="S37" si="7">AE37/$AJ$8</f>
         <v>22.207062014338497</v>
       </c>
       <c r="T37" s="20">
-        <f t="shared" ref="T37" si="8">Y37/$AC$8</f>
+        <f t="shared" ref="T37" si="8">AF37/$AJ$8</f>
         <v>22.91204811003178</v>
       </c>
-      <c r="V37">
+      <c r="U37" s="51"/>
+      <c r="V37" s="51"/>
+      <c r="W37" s="51"/>
+      <c r="X37" s="51"/>
+      <c r="Y37" s="51"/>
+      <c r="Z37" s="51"/>
+      <c r="AA37" s="51"/>
+      <c r="AC37">
         <f>19.2-7</f>
         <v>12.2</v>
       </c>
-      <c r="W37">
+      <c r="AD37">
         <f>19.9-7</f>
         <v>12.899999999999999</v>
       </c>
-      <c r="X37">
+      <c r="AE37">
         <f>20.3-7.7</f>
         <v>12.600000000000001</v>
       </c>
-      <c r="Y37">
+      <c r="AF37">
         <f>20-7</f>
         <v>13</v>
       </c>
     </row>
-    <row r="38" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A38" s="13"/>
       <c r="F38">
         <v>15</v>
@@ -2328,8 +2441,15 @@
       <c r="R38" s="21"/>
       <c r="S38" s="21"/>
       <c r="T38" s="22"/>
-    </row>
-    <row r="39" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="U38" s="52"/>
+      <c r="V38" s="52"/>
+      <c r="W38" s="52"/>
+      <c r="X38" s="52"/>
+      <c r="Y38" s="52"/>
+      <c r="Z38" s="52"/>
+      <c r="AA38" s="52"/>
+    </row>
+    <row r="39" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A39" s="13"/>
       <c r="F39">
         <v>15</v>
@@ -2353,11 +2473,11 @@
         <v>25</v>
       </c>
       <c r="Q39" s="19">
-        <f>V39/$AC$7</f>
+        <f>AC39/$AJ$7</f>
         <v>22.304701336891547</v>
       </c>
       <c r="R39" s="19">
-        <f t="shared" ref="R39:T39" si="9">W39/$AC$7</f>
+        <f t="shared" ref="R39:T39" si="9">AD39/$AJ$7</f>
         <v>23.001723253669407</v>
       </c>
       <c r="S39" s="19">
@@ -2368,27 +2488,34 @@
         <f t="shared" si="9"/>
         <v>24.395767087225131</v>
       </c>
-      <c r="V39">
+      <c r="U39" s="51"/>
+      <c r="V39" s="51"/>
+      <c r="W39" s="51"/>
+      <c r="X39" s="51"/>
+      <c r="Y39" s="51"/>
+      <c r="Z39" s="51"/>
+      <c r="AA39" s="51"/>
+      <c r="AC39">
         <f>9.5+6.5</f>
         <v>16</v>
       </c>
-      <c r="W39">
+      <c r="AD39">
         <f>9.5+7</f>
         <v>16.5</v>
       </c>
-      <c r="X39">
+      <c r="AE39">
         <f>10.1+7.1</f>
         <v>17.2</v>
       </c>
-      <c r="Y39">
+      <c r="AF39">
         <f>7.5+10</f>
         <v>17.5</v>
       </c>
-      <c r="Z39" t="s">
+      <c r="AG39" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="40" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A40" s="13"/>
       <c r="F40">
         <v>15</v>
@@ -2412,39 +2539,46 @@
         <v>21.14</v>
       </c>
       <c r="Q40" s="19">
-        <f>V40/$AC$7</f>
+        <f>AC40/$AJ$7</f>
         <v>21.607679420113687</v>
       </c>
       <c r="R40" s="19">
-        <f t="shared" ref="R40" si="10">W40/$AC$7</f>
+        <f t="shared" ref="R40" si="10">AD40/$AJ$7</f>
         <v>23.001723253669407</v>
       </c>
       <c r="S40" s="19">
-        <f t="shared" ref="S40" si="11">X40/$AC$7</f>
+        <f t="shared" ref="S40" si="11">AE40/$AJ$7</f>
         <v>23.419936403736127</v>
       </c>
       <c r="T40" s="20">
-        <f t="shared" ref="T40" si="12">Y40/$AC$7</f>
+        <f t="shared" ref="T40" si="12">AF40/$AJ$7</f>
         <v>24.116958320513987</v>
       </c>
-      <c r="V40">
+      <c r="U40" s="51"/>
+      <c r="V40" s="51"/>
+      <c r="W40" s="51"/>
+      <c r="X40" s="51"/>
+      <c r="Y40" s="51"/>
+      <c r="Z40" s="51"/>
+      <c r="AA40" s="51"/>
+      <c r="AC40">
         <f>21-5.5</f>
         <v>15.5</v>
       </c>
-      <c r="W40">
+      <c r="AD40">
         <f>21.5-5</f>
         <v>16.5</v>
       </c>
-      <c r="X40">
+      <c r="AE40">
         <f>23.5-6.7</f>
         <v>16.8</v>
       </c>
-      <c r="Y40">
+      <c r="AF40">
         <f>24.8-7.5</f>
         <v>17.3</v>
       </c>
     </row>
-    <row r="41" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A41" s="13"/>
       <c r="F41">
         <v>15</v>
@@ -2454,14 +2588,21 @@
       <c r="R41" s="21"/>
       <c r="S41" s="21"/>
       <c r="T41" s="22"/>
-      <c r="V41" s="2">
+      <c r="U41" s="52"/>
+      <c r="V41" s="52"/>
+      <c r="W41" s="52"/>
+      <c r="X41" s="52"/>
+      <c r="Y41" s="52"/>
+      <c r="Z41" s="52"/>
+      <c r="AA41" s="52"/>
+      <c r="AC41" s="2">
         <v>0.7</v>
       </c>
-      <c r="X41" s="2">
+      <c r="AE41" s="2">
         <v>0.8</v>
       </c>
     </row>
-    <row r="42" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A42" s="13"/>
       <c r="F42">
         <v>15</v>
@@ -2485,39 +2626,46 @@
         <v>25</v>
       </c>
       <c r="Q42" s="19">
-        <f>V42/$AC$7</f>
+        <f>AC42/$AJ$7</f>
         <v>23.698745170447268</v>
       </c>
       <c r="R42" s="19">
-        <f>W42/$AC$7</f>
+        <f>AD42/$AJ$7</f>
         <v>24.395767087225131</v>
       </c>
       <c r="S42" s="19">
-        <f>X42/$AC$8</f>
+        <f>AE42/$AJ$8</f>
         <v>24.674513349264995</v>
       </c>
       <c r="T42" s="20">
-        <f>Y42/$AC$8</f>
+        <f>AF42/$AJ$8</f>
         <v>25.203252921034959</v>
       </c>
-      <c r="V42">
+      <c r="U42" s="51"/>
+      <c r="V42" s="51"/>
+      <c r="W42" s="51"/>
+      <c r="X42" s="51"/>
+      <c r="Y42" s="51"/>
+      <c r="Z42" s="51"/>
+      <c r="AA42" s="51"/>
+      <c r="AC42">
         <f>17</f>
         <v>17</v>
       </c>
-      <c r="W42">
+      <c r="AD42">
         <f>17.5</f>
         <v>17.5</v>
       </c>
-      <c r="X42">
+      <c r="AE42">
         <f>6+8</f>
         <v>14</v>
       </c>
-      <c r="Y42">
+      <c r="AF42">
         <f>6+8.3</f>
         <v>14.3</v>
       </c>
     </row>
-    <row r="43" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A43" s="13"/>
       <c r="F43">
         <v>15</v>
@@ -2541,39 +2689,46 @@
         <v>23.32</v>
       </c>
       <c r="Q43" s="19">
-        <f>V43/$AC$7</f>
+        <f>AC43/$AJ$7</f>
         <v>20.910657503335827</v>
       </c>
       <c r="R43" s="19">
-        <f>W43/$AC$7</f>
+        <f>AD43/$AJ$7</f>
         <v>23.001723253669407</v>
       </c>
       <c r="S43" s="19">
-        <f>X43/$AC$8</f>
+        <f>AE43/$AJ$8</f>
         <v>20.26835025118196</v>
       </c>
       <c r="T43" s="20">
-        <f>Y43/$AC$8</f>
+        <f>AF43/$AJ$8</f>
         <v>22.383308538261815</v>
       </c>
-      <c r="V43">
+      <c r="U43" s="51"/>
+      <c r="V43" s="51"/>
+      <c r="W43" s="51"/>
+      <c r="X43" s="51"/>
+      <c r="Y43" s="51"/>
+      <c r="Z43" s="51"/>
+      <c r="AA43" s="51"/>
+      <c r="AC43">
         <f>20.5-5.5</f>
         <v>15</v>
       </c>
-      <c r="W43">
+      <c r="AD43">
         <f>22.8-6.3</f>
         <v>16.5</v>
       </c>
-      <c r="X43">
+      <c r="AE43">
         <f>18.5-7</f>
         <v>11.5</v>
       </c>
-      <c r="Y43">
+      <c r="AF43">
         <f>19.7-7</f>
         <v>12.7</v>
       </c>
     </row>
-    <row r="44" spans="1:26" s="33" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:33" s="33" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="32"/>
       <c r="F44" s="33">
         <v>15</v>
@@ -2583,7 +2738,7 @@
       <c r="O44" s="32"/>
       <c r="T44" s="34"/>
     </row>
-    <row r="45" spans="1:26" s="30" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:33" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A45" s="29"/>
       <c r="B45" s="30" t="s">
         <v>0</v>
@@ -2604,7 +2759,7 @@
       <c r="O45" s="29"/>
       <c r="T45" s="31"/>
     </row>
-    <row r="46" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A46" s="13"/>
       <c r="E46">
         <v>1</v>
@@ -2612,11 +2767,11 @@
       <c r="F46">
         <v>8</v>
       </c>
-      <c r="X46" s="2">
+      <c r="AE46" s="2">
         <v>0.6</v>
       </c>
     </row>
-    <row r="47" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A47" s="13"/>
       <c r="E47">
         <v>1</v>
@@ -2665,23 +2820,30 @@
         <v>17.5</v>
       </c>
       <c r="S47" s="17">
-        <f>X47/$AC$6</f>
+        <f>AE47/$AJ$6</f>
         <v>20.268688198693614</v>
       </c>
       <c r="T47" s="18">
-        <f>Y47/$AC$6</f>
+        <f>AF47/$AJ$6</f>
         <v>21.200581908978378</v>
       </c>
-      <c r="X47">
+      <c r="U47" s="50"/>
+      <c r="V47" s="50"/>
+      <c r="W47" s="50"/>
+      <c r="X47" s="50"/>
+      <c r="Y47" s="50"/>
+      <c r="Z47" s="50"/>
+      <c r="AA47" s="50"/>
+      <c r="AE47">
         <f>20.7-3.3</f>
         <v>17.399999999999999</v>
       </c>
-      <c r="Y47">
+      <c r="AF47">
         <f>21.5-3.3</f>
         <v>18.2</v>
       </c>
     </row>
-    <row r="48" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A48" s="13"/>
       <c r="E48">
         <v>1</v>
@@ -2730,23 +2892,30 @@
         <v>19</v>
       </c>
       <c r="S48" s="17">
-        <f>X48/$AC$6</f>
+        <f>AE48/$AJ$6</f>
         <v>20.035714771122425</v>
       </c>
       <c r="T48" s="18">
-        <f>Y48/$AC$6</f>
+        <f>AF48/$AJ$6</f>
         <v>20.851121767621596</v>
       </c>
-      <c r="X48">
+      <c r="U48" s="50"/>
+      <c r="V48" s="50"/>
+      <c r="W48" s="50"/>
+      <c r="X48" s="50"/>
+      <c r="Y48" s="50"/>
+      <c r="Z48" s="50"/>
+      <c r="AA48" s="50"/>
+      <c r="AE48">
         <f>20.5-3.3</f>
         <v>17.2</v>
       </c>
-      <c r="Y48">
+      <c r="AF48">
         <f>21.3-3.4</f>
         <v>17.900000000000002</v>
       </c>
     </row>
-    <row r="49" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A49" s="13"/>
       <c r="E49">
         <v>1</v>
@@ -2760,7 +2929,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="50" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A50" s="13"/>
       <c r="E50">
         <v>1</v>
@@ -2793,7 +2962,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="51" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A51" s="13"/>
       <c r="E51">
         <v>1</v>
@@ -2826,7 +2995,7 @@
         <v>24.62</v>
       </c>
     </row>
-    <row r="52" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A52" s="13"/>
       <c r="E52">
         <v>1</v>
@@ -2838,14 +3007,14 @@
       <c r="I52" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="V52" s="2">
+      <c r="AC52" s="2">
         <v>0.6</v>
       </c>
-      <c r="Y52" s="2">
+      <c r="AF52" s="2">
         <v>0.7</v>
       </c>
     </row>
-    <row r="53" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A53" s="13"/>
       <c r="E53">
         <v>1</v>
@@ -2872,39 +3041,46 @@
         <v>20.34</v>
       </c>
       <c r="Q53" s="17">
-        <f>V53/$AC$6</f>
+        <f>AC53/$AJ$6</f>
         <v>15.725706361055392</v>
       </c>
       <c r="R53" s="17">
-        <f>W53/$AC$6</f>
+        <f>AD53/$AJ$6</f>
         <v>16.075166502412181</v>
       </c>
       <c r="S53" s="17">
-        <f>X53/$AC$6</f>
+        <f>AE53/$AJ$6</f>
         <v>16.308139929983369</v>
       </c>
       <c r="T53" s="18">
-        <f>Y53/$AC$7</f>
+        <f>AF53/$AJ$7</f>
         <v>17.146739152735378</v>
       </c>
-      <c r="V53">
+      <c r="U53" s="50"/>
+      <c r="V53" s="50"/>
+      <c r="W53" s="50"/>
+      <c r="X53" s="50"/>
+      <c r="Y53" s="50"/>
+      <c r="Z53" s="50"/>
+      <c r="AA53" s="50"/>
+      <c r="AC53">
         <f>8+5.5</f>
         <v>13.5</v>
       </c>
-      <c r="W53">
+      <c r="AD53">
         <f>8+5.8</f>
         <v>13.8</v>
       </c>
-      <c r="X53">
+      <c r="AE53">
         <f>8+6</f>
         <v>14</v>
       </c>
-      <c r="Y53">
+      <c r="AF53">
         <f>7+5.3</f>
         <v>12.3</v>
       </c>
     </row>
-    <row r="54" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A54" s="13"/>
       <c r="E54">
         <v>1</v>
@@ -2931,39 +3107,46 @@
         <v>19.3</v>
       </c>
       <c r="Q54" s="17">
-        <f>V54/$AC$6</f>
+        <f>AC54/$AJ$6</f>
         <v>19.802741343551233</v>
       </c>
       <c r="R54" s="17">
-        <f t="shared" ref="R54" si="13">W54/$AC$6</f>
+        <f t="shared" ref="R54" si="13">AD54/$AJ$6</f>
         <v>20.385174912479211</v>
       </c>
       <c r="S54" s="17">
-        <f t="shared" ref="S54" si="14">X54/$AC$6</f>
+        <f t="shared" ref="S54" si="14">AE54/$AJ$6</f>
         <v>20.152201484908023</v>
       </c>
       <c r="T54" s="18">
-        <f>Y54/$AC$7</f>
+        <f>AF54/$AJ$7</f>
         <v>20.631848736624683</v>
       </c>
-      <c r="V54">
+      <c r="U54" s="50"/>
+      <c r="V54" s="50"/>
+      <c r="W54" s="50"/>
+      <c r="X54" s="50"/>
+      <c r="Y54" s="50"/>
+      <c r="Z54" s="50"/>
+      <c r="AA54" s="50"/>
+      <c r="AC54">
         <f>20-3</f>
         <v>17</v>
       </c>
-      <c r="W54">
+      <c r="AD54">
         <f>20.7-3.2</f>
         <v>17.5</v>
       </c>
-      <c r="X54">
+      <c r="AE54">
         <f>20.3-3</f>
         <v>17.3</v>
       </c>
-      <c r="Y54">
+      <c r="AF54">
         <f>18-3.2</f>
         <v>14.8</v>
       </c>
     </row>
-    <row r="55" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A55" s="13"/>
       <c r="E55">
         <v>1</v>
@@ -2975,14 +3158,14 @@
       <c r="I55" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="V55" s="2">
+      <c r="AC55" s="2">
         <v>0.6</v>
       </c>
-      <c r="W55" s="2">
+      <c r="AD55" s="2">
         <v>0.7</v>
       </c>
     </row>
-    <row r="56" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A56" s="13"/>
       <c r="E56">
         <v>1</v>
@@ -3009,11 +3192,11 @@
         <v>25</v>
       </c>
       <c r="Q56" s="17">
-        <f>V56/$AC$6</f>
+        <f>AC56/$AJ$6</f>
         <v>16.191653216197775</v>
       </c>
       <c r="R56" s="17">
-        <f t="shared" ref="R56:T57" si="15">W56/$AC$7</f>
+        <f t="shared" ref="R56:T57" si="15">AD56/$AJ$7</f>
         <v>16.728526002668662</v>
       </c>
       <c r="S56" s="17">
@@ -3024,24 +3207,31 @@
         <f t="shared" si="15"/>
         <v>21.328870653402543</v>
       </c>
-      <c r="V56">
+      <c r="U56" s="50"/>
+      <c r="V56" s="50"/>
+      <c r="W56" s="50"/>
+      <c r="X56" s="50"/>
+      <c r="Y56" s="50"/>
+      <c r="Z56" s="50"/>
+      <c r="AA56" s="50"/>
+      <c r="AC56">
         <f>7.5+6.4</f>
         <v>13.9</v>
       </c>
-      <c r="W56">
+      <c r="AD56">
         <f>6.5+5.5</f>
         <v>12</v>
       </c>
-      <c r="X56">
+      <c r="AE56">
         <f>7+6.5</f>
         <v>13.5</v>
       </c>
-      <c r="Y56">
+      <c r="AF56">
         <f>7.3+8</f>
         <v>15.3</v>
       </c>
     </row>
-    <row r="57" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A57" s="13"/>
       <c r="E57">
         <v>1</v>
@@ -3068,7 +3258,7 @@
         <v>22.8799999999999</v>
       </c>
       <c r="Q57" s="17">
-        <f>V57/$AC$6</f>
+        <f>AC57/$AJ$6</f>
         <v>18.63787420569528</v>
       </c>
       <c r="R57" s="17">
@@ -3083,24 +3273,31 @@
         <f t="shared" si="15"/>
         <v>26.486832837558712</v>
       </c>
-      <c r="V57">
+      <c r="U57" s="50"/>
+      <c r="V57" s="50"/>
+      <c r="W57" s="50"/>
+      <c r="X57" s="50"/>
+      <c r="Y57" s="50"/>
+      <c r="Z57" s="50"/>
+      <c r="AA57" s="50"/>
+      <c r="AC57">
         <f>19.2-3.2</f>
         <v>16</v>
       </c>
-      <c r="W57">
+      <c r="AD57">
         <f>19-3.5</f>
         <v>15.5</v>
       </c>
-      <c r="X57">
+      <c r="AE57">
         <f>21-4</f>
         <v>17</v>
       </c>
-      <c r="Y57">
+      <c r="AF57">
         <f>23-4</f>
         <v>19</v>
       </c>
     </row>
-    <row r="58" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A58" s="13"/>
       <c r="E58">
         <v>1</v>
@@ -3110,7 +3307,7 @@
       </c>
       <c r="H58" s="11"/>
     </row>
-    <row r="59" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A59" s="13"/>
       <c r="E59">
         <v>2</v>
@@ -3119,7 +3316,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="60" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A60" s="13"/>
       <c r="E60">
         <v>2</v>
@@ -3127,14 +3324,14 @@
       <c r="F60">
         <v>8</v>
       </c>
-      <c r="X60" s="2">
+      <c r="AE60" s="2">
         <v>0.6</v>
       </c>
-      <c r="Y60" s="2">
+      <c r="AF60" s="2">
         <v>0.7</v>
       </c>
     </row>
-    <row r="61" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A61" s="13"/>
       <c r="E61">
         <v>2</v>
@@ -3177,23 +3374,30 @@
         <v>18.799999999999997</v>
       </c>
       <c r="S61" s="17">
-        <f>X61/AC6</f>
+        <f>AE61/AJ6</f>
         <v>21.550042050335168</v>
       </c>
       <c r="T61" s="18">
-        <f>Y61/AC7</f>
+        <f>AF61/AJ7</f>
         <v>19.934826819846823</v>
       </c>
-      <c r="X61">
+      <c r="U61" s="50"/>
+      <c r="V61" s="50"/>
+      <c r="W61" s="50"/>
+      <c r="X61" s="50"/>
+      <c r="Y61" s="50"/>
+      <c r="Z61" s="50"/>
+      <c r="AA61" s="50"/>
+      <c r="AE61">
         <f>20.3-1.8</f>
         <v>18.5</v>
       </c>
-      <c r="Y61">
+      <c r="AF61">
         <f>16.3-2</f>
         <v>14.3</v>
       </c>
     </row>
-    <row r="62" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A62" s="13"/>
       <c r="E62">
         <v>2</v>
@@ -3236,23 +3440,30 @@
         <v>17.5</v>
       </c>
       <c r="S62" s="17">
-        <f>X62/AC6</f>
+        <f>AE62/AJ6</f>
         <v>20.268688198693614</v>
       </c>
       <c r="T62" s="18">
-        <f>Y62/AC7</f>
+        <f>AF62/AJ7</f>
         <v>21.468275036758115</v>
       </c>
-      <c r="X62">
+      <c r="U62" s="50"/>
+      <c r="V62" s="50"/>
+      <c r="W62" s="50"/>
+      <c r="X62" s="50"/>
+      <c r="Y62" s="50"/>
+      <c r="Z62" s="50"/>
+      <c r="AA62" s="50"/>
+      <c r="AE62">
         <f>9+8.4</f>
         <v>17.399999999999999</v>
       </c>
-      <c r="Y62">
+      <c r="AF62">
         <f>7.5+7.9</f>
         <v>15.4</v>
       </c>
     </row>
-    <row r="63" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A63" s="13"/>
       <c r="E63">
         <v>2</v>
@@ -3262,11 +3473,11 @@
       </c>
       <c r="G63" s="11"/>
       <c r="H63" s="11"/>
-      <c r="V63" s="2">
+      <c r="AC63" s="2">
         <v>0.7</v>
       </c>
     </row>
-    <row r="64" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A64" s="13"/>
       <c r="E64">
         <v>2</v>
@@ -3294,18 +3505,18 @@
         <v>23.079999999999899</v>
       </c>
       <c r="O64" s="23">
-        <f>V64/AC7</f>
+        <f>AC64/AJ7</f>
         <v>18.401378602935527</v>
       </c>
       <c r="P64" s="24" t="s">
         <v>9</v>
       </c>
       <c r="Q64" s="17">
-        <f>W64/$AC$7</f>
+        <f>AD64/$AJ$7</f>
         <v>19.934826819846823</v>
       </c>
       <c r="R64" s="17">
-        <f t="shared" ref="R64:T64" si="16">X64/$AC$7</f>
+        <f t="shared" ref="R64:T64" si="16">AE64/$AJ$7</f>
         <v>21.050061886691399</v>
       </c>
       <c r="S64" s="17">
@@ -3316,28 +3527,35 @@
         <f t="shared" si="16"/>
         <v>24.116958320513987</v>
       </c>
-      <c r="V64">
+      <c r="U64" s="50"/>
+      <c r="V64" s="50"/>
+      <c r="W64" s="50"/>
+      <c r="X64" s="50"/>
+      <c r="Y64" s="50"/>
+      <c r="Z64" s="50"/>
+      <c r="AA64" s="50"/>
+      <c r="AC64">
         <f>6.5+6.7</f>
         <v>13.2</v>
       </c>
-      <c r="W64">
+      <c r="AD64">
         <f>7.5+6.8</f>
         <v>14.3</v>
       </c>
-      <c r="X64">
+      <c r="AE64">
         <f>8+7.1</f>
         <v>15.1</v>
       </c>
-      <c r="Y64">
+      <c r="AF64">
         <f>8.6+8.4</f>
         <v>17</v>
       </c>
-      <c r="Z64">
+      <c r="AG64">
         <f>8.8+8.5</f>
         <v>17.3</v>
       </c>
     </row>
-    <row r="65" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A65" s="13"/>
       <c r="E65">
         <v>2</v>
@@ -3365,50 +3583,57 @@
         <v>20.32</v>
       </c>
       <c r="O65" s="23">
-        <f>V65/AC7</f>
+        <f>AC65/AJ7</f>
         <v>23.698745170447268</v>
       </c>
       <c r="P65" s="24" t="s">
         <v>9</v>
       </c>
       <c r="Q65" s="17">
-        <f>W65/$AC$7</f>
+        <f>AD65/$AJ$7</f>
         <v>22.862318870313835</v>
       </c>
       <c r="R65" s="17">
-        <f t="shared" ref="R65" si="17">X65/$AC$7</f>
+        <f t="shared" ref="R65" si="17">AE65/$AJ$7</f>
         <v>23.419936403736127</v>
       </c>
       <c r="S65" s="17">
-        <f t="shared" ref="S65" si="18">Y65/$AC$7</f>
+        <f t="shared" ref="S65" si="18">AF65/$AJ$7</f>
         <v>21.050061886691399</v>
       </c>
       <c r="T65" s="18">
-        <f t="shared" ref="T65" si="19">Z65/$AC$7</f>
+        <f t="shared" ref="T65" si="19">AG65/$AJ$7</f>
         <v>18.680187369646667</v>
       </c>
-      <c r="V65">
+      <c r="U65" s="50"/>
+      <c r="V65" s="50"/>
+      <c r="W65" s="50"/>
+      <c r="X65" s="50"/>
+      <c r="Y65" s="50"/>
+      <c r="Z65" s="50"/>
+      <c r="AA65" s="50"/>
+      <c r="AC65">
         <f>19-2</f>
         <v>17</v>
       </c>
-      <c r="W65">
+      <c r="AD65">
         <f>19-2.6</f>
         <v>16.399999999999999</v>
       </c>
-      <c r="X65">
+      <c r="AE65">
         <f>19.5-2.7</f>
         <v>16.8</v>
       </c>
-      <c r="Y65">
+      <c r="AF65">
         <f>18.3-3.2</f>
         <v>15.100000000000001</v>
       </c>
-      <c r="Z65">
+      <c r="AG65">
         <f>16.7-3.3</f>
         <v>13.399999999999999</v>
       </c>
     </row>
-    <row r="66" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A66" s="13"/>
       <c r="E66">
         <v>2</v>
@@ -3418,7 +3643,7 @@
       </c>
       <c r="H66" s="11"/>
     </row>
-    <row r="67" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A67" s="13"/>
       <c r="E67">
         <v>2</v>
@@ -3453,26 +3678,33 @@
         <v>15.5</v>
       </c>
       <c r="S67" s="17">
-        <f>X67/$AC$6</f>
+        <f>AE67/$AJ$6</f>
         <v>15.842193074840988</v>
       </c>
       <c r="T67" s="18">
-        <f>Y67/$AC$6</f>
+        <f>AF67/$AJ$6</f>
         <v>16.657600071340156</v>
       </c>
-      <c r="W67" t="s">
+      <c r="U67" s="50"/>
+      <c r="V67" s="50"/>
+      <c r="W67" s="50"/>
+      <c r="X67" s="50"/>
+      <c r="Y67" s="50"/>
+      <c r="Z67" s="50"/>
+      <c r="AA67" s="50"/>
+      <c r="AD67" t="s">
         <v>24</v>
       </c>
-      <c r="X67">
+      <c r="AE67">
         <f>7.4+6.2</f>
         <v>13.600000000000001</v>
       </c>
-      <c r="Y67">
+      <c r="AF67">
         <f>8+6.3</f>
         <v>14.3</v>
       </c>
     </row>
-    <row r="68" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A68" s="13"/>
       <c r="E68">
         <v>2</v>
@@ -3507,23 +3739,30 @@
         <v>19</v>
       </c>
       <c r="S68" s="17">
-        <f>X68/$AC$6</f>
+        <f>AE68/$AJ$6</f>
         <v>18.870847633266468</v>
       </c>
       <c r="T68" s="18">
-        <f>Y68/$AC$6</f>
+        <f>AF68/$AJ$6</f>
         <v>21.666528764120759</v>
       </c>
-      <c r="X68">
+      <c r="U68" s="50"/>
+      <c r="V68" s="50"/>
+      <c r="W68" s="50"/>
+      <c r="X68" s="50"/>
+      <c r="Y68" s="50"/>
+      <c r="Z68" s="50"/>
+      <c r="AA68" s="50"/>
+      <c r="AE68">
         <f>17.7-1.5</f>
         <v>16.2</v>
       </c>
-      <c r="Y68">
+      <c r="AF68">
         <f>20.2-1.6</f>
         <v>18.599999999999998</v>
       </c>
     </row>
-    <row r="69" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A69" s="13"/>
       <c r="E69">
         <v>2</v>
@@ -3532,20 +3771,20 @@
         <v>8</v>
       </c>
       <c r="H69" s="11"/>
-      <c r="V69" s="9">
+      <c r="AC69" s="9">
         <v>0.6</v>
       </c>
-      <c r="W69" s="9">
+      <c r="AD69" s="9">
         <v>0.7</v>
       </c>
-      <c r="X69" s="9">
+      <c r="AE69" s="9">
         <v>0.8</v>
       </c>
-      <c r="Y69" s="9">
+      <c r="AF69" s="9">
         <v>0.8</v>
       </c>
     </row>
-    <row r="70" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A70" s="13"/>
       <c r="E70">
         <v>2</v>
@@ -3575,24 +3814,31 @@
       <c r="R70" s="25"/>
       <c r="S70" s="25"/>
       <c r="T70" s="26"/>
-      <c r="V70">
+      <c r="U70" s="53"/>
+      <c r="V70" s="53"/>
+      <c r="W70" s="53"/>
+      <c r="X70" s="53"/>
+      <c r="Y70" s="53"/>
+      <c r="Z70" s="53"/>
+      <c r="AA70" s="53"/>
+      <c r="AC70">
         <f>7.3+5.5</f>
         <v>12.8</v>
       </c>
-      <c r="W70">
+      <c r="AD70">
         <f>7.2+5.5</f>
         <v>12.7</v>
       </c>
-      <c r="X70">
+      <c r="AE70">
         <f>5.3+4.9</f>
         <v>10.199999999999999</v>
       </c>
-      <c r="Y70">
+      <c r="AF70">
         <f>5.5+5.5</f>
         <v>11</v>
       </c>
     </row>
-    <row r="71" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A71" s="13"/>
       <c r="E71">
         <v>2</v>
@@ -3619,39 +3865,46 @@
         <v>28.16</v>
       </c>
       <c r="Q71" s="17">
-        <f>V71/AC6</f>
+        <f>AC71/AJ6</f>
         <v>18.171927350552899</v>
       </c>
       <c r="R71" s="17">
-        <f>W71/AC7</f>
+        <f>AD71/AJ7</f>
         <v>23.977553937158412</v>
       </c>
       <c r="S71" s="17">
-        <f>X71/$AC$8</f>
+        <f>AE71/$AJ$8</f>
         <v>23.793280729648387</v>
       </c>
       <c r="T71" s="18">
-        <f>Y71/$AC$8</f>
+        <f>AF71/$AJ$8</f>
         <v>26.436978588498206</v>
       </c>
-      <c r="V71">
+      <c r="U71" s="50"/>
+      <c r="V71" s="50"/>
+      <c r="W71" s="50"/>
+      <c r="X71" s="50"/>
+      <c r="Y71" s="50"/>
+      <c r="Z71" s="50"/>
+      <c r="AA71" s="50"/>
+      <c r="AC71">
         <f>17-1.4</f>
         <v>15.6</v>
       </c>
-      <c r="W71">
+      <c r="AD71">
         <f>19-1.8</f>
         <v>17.2</v>
       </c>
-      <c r="X71">
+      <c r="AE71">
         <f>15.8-2.3</f>
         <v>13.5</v>
       </c>
-      <c r="Y71">
+      <c r="AF71">
         <f>17.9-2.9</f>
         <v>14.999999999999998</v>
       </c>
     </row>
-    <row r="72" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A72" s="13"/>
       <c r="E72">
         <v>2</v>
@@ -3661,7 +3914,7 @@
       </c>
       <c r="H72" s="11"/>
     </row>
-    <row r="73" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A73" s="13"/>
       <c r="E73">
         <v>2</v>
@@ -3670,7 +3923,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="74" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A74" s="13"/>
       <c r="E74">
         <v>2</v>
@@ -3700,7 +3953,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="75" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A75" s="13"/>
       <c r="E75">
         <v>2</v>
@@ -3727,7 +3980,7 @@
         <v>27.559999999999899</v>
       </c>
     </row>
-    <row r="76" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A76" s="13"/>
       <c r="E76">
         <v>2</v>
@@ -3737,7 +3990,7 @@
       </c>
       <c r="G76" s="11"/>
     </row>
-    <row r="77" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A77" s="13"/>
       <c r="E77">
         <v>2</v>
@@ -3764,7 +4017,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="78" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A78" s="13"/>
       <c r="E78">
         <v>2</v>
@@ -3791,7 +4044,7 @@
         <v>27.72</v>
       </c>
     </row>
-    <row r="79" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A79" s="13"/>
       <c r="E79">
         <v>2</v>
@@ -3800,7 +4053,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="80" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A80" s="13"/>
       <c r="E80">
         <v>2</v>
@@ -3827,7 +4080,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="81" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A81" s="13"/>
       <c r="E81">
         <v>2</v>
@@ -3854,7 +4107,7 @@
         <v>25.94</v>
       </c>
     </row>
-    <row r="82" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A82" s="13"/>
       <c r="E82">
         <v>2</v>
@@ -3863,7 +4116,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="83" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A83" s="13"/>
       <c r="E83">
         <v>2</v>
@@ -3890,7 +4143,7 @@
         <v>26.64</v>
       </c>
     </row>
-    <row r="84" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A84" s="13"/>
       <c r="E84">
         <v>2</v>
@@ -3917,7 +4170,7 @@
         <v>27.239999999999899</v>
       </c>
     </row>
-    <row r="85" spans="1:23" s="33" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:30" s="33" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A85" s="32"/>
       <c r="E85" s="33">
         <v>2</v>
@@ -3929,7 +4182,7 @@
       <c r="O85" s="32"/>
       <c r="T85" s="34"/>
     </row>
-    <row r="86" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B86" t="s">
         <v>1</v>
       </c>
@@ -3946,7 +4199,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="87" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:30" x14ac:dyDescent="0.3">
       <c r="E87">
         <v>1</v>
       </c>
@@ -3957,7 +4210,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="88" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:30" x14ac:dyDescent="0.3">
       <c r="E88">
         <v>1</v>
       </c>
@@ -4013,7 +4266,7 @@
         <v>18.7</v>
       </c>
     </row>
-    <row r="89" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:30" x14ac:dyDescent="0.3">
       <c r="E89">
         <v>1</v>
       </c>
@@ -4069,7 +4322,7 @@
         <v>11.600000000000001</v>
       </c>
     </row>
-    <row r="90" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:30" x14ac:dyDescent="0.3">
       <c r="E90">
         <v>1</v>
       </c>
@@ -4081,9 +4334,9 @@
       <c r="I90" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="W90" s="2"/>
-    </row>
-    <row r="91" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="AD90" s="2"/>
+    </row>
+    <row r="91" spans="1:30" x14ac:dyDescent="0.3">
       <c r="E91">
         <v>1</v>
       </c>
@@ -4139,7 +4392,7 @@
         <v>20.5</v>
       </c>
     </row>
-    <row r="92" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:30" x14ac:dyDescent="0.3">
       <c r="E92">
         <v>1</v>
       </c>
@@ -4195,7 +4448,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="93" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:30" x14ac:dyDescent="0.3">
       <c r="E93">
         <v>1</v>
       </c>
@@ -4207,7 +4460,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="94" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:30" x14ac:dyDescent="0.3">
       <c r="E94">
         <v>1</v>
       </c>
@@ -4263,7 +4516,7 @@
         <v>14.4</v>
       </c>
     </row>
-    <row r="95" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:30" x14ac:dyDescent="0.3">
       <c r="E95">
         <v>1</v>
       </c>
@@ -4319,7 +4572,7 @@
         <v>11.200000000000001</v>
       </c>
     </row>
-    <row r="96" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:30" x14ac:dyDescent="0.3">
       <c r="E96">
         <v>1</v>
       </c>
@@ -4331,7 +4584,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="97" spans="5:23" x14ac:dyDescent="0.3">
+    <row r="97" spans="5:30" x14ac:dyDescent="0.3">
       <c r="E97">
         <v>1</v>
       </c>
@@ -4387,7 +4640,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="98" spans="5:23" x14ac:dyDescent="0.3">
+    <row r="98" spans="5:30" x14ac:dyDescent="0.3">
       <c r="E98">
         <v>1</v>
       </c>
@@ -4442,8 +4695,15 @@
         <f>18.7-1.7</f>
         <v>17</v>
       </c>
-    </row>
-    <row r="99" spans="5:23" x14ac:dyDescent="0.3">
+      <c r="U98" s="54"/>
+      <c r="V98" s="54"/>
+      <c r="W98" s="54"/>
+      <c r="X98" s="54"/>
+      <c r="Y98" s="54"/>
+      <c r="Z98" s="54"/>
+      <c r="AA98" s="54"/>
+    </row>
+    <row r="99" spans="5:30" x14ac:dyDescent="0.3">
       <c r="E99">
         <v>1</v>
       </c>
@@ -4451,7 +4711,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="100" spans="5:23" x14ac:dyDescent="0.3">
+    <row r="100" spans="5:30" x14ac:dyDescent="0.3">
       <c r="E100">
         <v>2</v>
       </c>
@@ -4459,7 +4719,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="101" spans="5:23" x14ac:dyDescent="0.3">
+    <row r="101" spans="5:30" x14ac:dyDescent="0.3">
       <c r="E101">
         <v>2</v>
       </c>
@@ -4467,7 +4727,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="102" spans="5:23" x14ac:dyDescent="0.3">
+    <row r="102" spans="5:30" x14ac:dyDescent="0.3">
       <c r="E102">
         <v>2</v>
       </c>
@@ -4509,7 +4769,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="103" spans="5:23" x14ac:dyDescent="0.3">
+    <row r="103" spans="5:30" x14ac:dyDescent="0.3">
       <c r="E103">
         <v>2</v>
       </c>
@@ -4551,7 +4811,7 @@
         <v>10.700000000000001</v>
       </c>
     </row>
-    <row r="104" spans="5:23" x14ac:dyDescent="0.3">
+    <row r="104" spans="5:30" x14ac:dyDescent="0.3">
       <c r="E104">
         <v>2</v>
       </c>
@@ -4560,11 +4820,11 @@
       </c>
       <c r="G104" s="11"/>
       <c r="H104" s="11"/>
-      <c r="W104" s="2">
+      <c r="AD104" s="2">
         <v>0.6</v>
       </c>
     </row>
-    <row r="105" spans="5:23" x14ac:dyDescent="0.3">
+    <row r="105" spans="5:30" x14ac:dyDescent="0.3">
       <c r="E105">
         <v>2</v>
       </c>
@@ -4602,15 +4862,22 @@
         <v>19.7</v>
       </c>
       <c r="T105" s="28">
-        <f>W105/AC6</f>
+        <f>AD105/AJ6</f>
         <v>21.666528764120763</v>
       </c>
-      <c r="W105">
+      <c r="U105" s="55"/>
+      <c r="V105" s="55"/>
+      <c r="W105" s="55"/>
+      <c r="X105" s="55"/>
+      <c r="Y105" s="55"/>
+      <c r="Z105" s="55"/>
+      <c r="AA105" s="55"/>
+      <c r="AD105">
         <f>8+10.6</f>
         <v>18.600000000000001</v>
       </c>
     </row>
-    <row r="106" spans="5:23" x14ac:dyDescent="0.3">
+    <row r="106" spans="5:30" x14ac:dyDescent="0.3">
       <c r="E106">
         <v>2</v>
       </c>
@@ -4652,7 +4919,7 @@
         <v>13.5</v>
       </c>
     </row>
-    <row r="107" spans="5:23" x14ac:dyDescent="0.3">
+    <row r="107" spans="5:30" x14ac:dyDescent="0.3">
       <c r="E107">
         <v>2</v>
       </c>
@@ -4661,7 +4928,7 @@
       </c>
       <c r="H107" s="11"/>
     </row>
-    <row r="108" spans="5:23" x14ac:dyDescent="0.3">
+    <row r="108" spans="5:30" x14ac:dyDescent="0.3">
       <c r="E108">
         <v>2</v>
       </c>
@@ -4703,7 +4970,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="109" spans="5:23" x14ac:dyDescent="0.3">
+    <row r="109" spans="5:30" x14ac:dyDescent="0.3">
       <c r="E109">
         <v>2</v>
       </c>
@@ -4745,7 +5012,7 @@
         <v>11.2</v>
       </c>
     </row>
-    <row r="110" spans="5:23" x14ac:dyDescent="0.3">
+    <row r="110" spans="5:30" x14ac:dyDescent="0.3">
       <c r="E110">
         <v>2</v>
       </c>
@@ -4754,7 +5021,7 @@
       </c>
       <c r="H110" s="11"/>
     </row>
-    <row r="111" spans="5:23" x14ac:dyDescent="0.3">
+    <row r="111" spans="5:30" x14ac:dyDescent="0.3">
       <c r="E111">
         <v>2</v>
       </c>
@@ -4796,7 +5063,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="112" spans="5:23" x14ac:dyDescent="0.3">
+    <row r="112" spans="5:30" x14ac:dyDescent="0.3">
       <c r="E112">
         <v>2</v>
       </c>
@@ -4838,7 +5105,7 @@
         <v>12.5</v>
       </c>
     </row>
-    <row r="113" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:32" x14ac:dyDescent="0.3">
       <c r="E113">
         <v>2</v>
       </c>
@@ -4846,7 +5113,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="114" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:32" x14ac:dyDescent="0.3">
       <c r="E114">
         <v>2</v>
       </c>
@@ -4854,18 +5121,18 @@
         <v>8</v>
       </c>
     </row>
-    <row r="115" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:32" x14ac:dyDescent="0.3">
       <c r="E115">
         <v>2</v>
       </c>
       <c r="F115">
         <v>8</v>
       </c>
-      <c r="V115" s="2">
+      <c r="AC115" s="2">
         <v>0.8</v>
       </c>
     </row>
-    <row r="116" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:32" x14ac:dyDescent="0.3">
       <c r="E116">
         <v>2</v>
       </c>
@@ -4891,11 +5158,11 @@
         <v>25</v>
       </c>
       <c r="Q116" s="19">
-        <f>V116/$AC$8</f>
+        <f>AC116/$AJ$8</f>
         <v>19.387117631565353</v>
       </c>
       <c r="R116" s="19">
-        <f t="shared" ref="R116:T116" si="20">W116/$AC$8</f>
+        <f t="shared" ref="R116:T116" si="20">AD116/$AJ$8</f>
         <v>21.149582870798568</v>
       </c>
       <c r="S116" s="19">
@@ -4906,24 +5173,31 @@
         <f t="shared" si="20"/>
         <v>23.969527253571709</v>
       </c>
-      <c r="V116">
+      <c r="U116" s="51"/>
+      <c r="V116" s="51"/>
+      <c r="W116" s="51"/>
+      <c r="X116" s="51"/>
+      <c r="Y116" s="51"/>
+      <c r="Z116" s="51"/>
+      <c r="AA116" s="51"/>
+      <c r="AC116">
         <f>7+4</f>
         <v>11</v>
       </c>
-      <c r="W116">
+      <c r="AD116">
         <f>7+5</f>
         <v>12</v>
       </c>
-      <c r="X116">
+      <c r="AE116">
         <f>7.7+5.5</f>
         <v>13.2</v>
       </c>
-      <c r="Y116">
+      <c r="AF116">
         <f>7.6+6</f>
         <v>13.6</v>
       </c>
     </row>
-    <row r="117" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:32" x14ac:dyDescent="0.3">
       <c r="E117">
         <v>2</v>
       </c>
@@ -4949,39 +5223,46 @@
         <v>24.6999999999999</v>
       </c>
       <c r="Q117" s="19">
-        <f>V117/$AC$8</f>
+        <f>AC117/$AJ$8</f>
         <v>21.149582870798568</v>
       </c>
       <c r="R117" s="19">
-        <f t="shared" ref="R117" si="21">W117/$AC$8</f>
+        <f t="shared" ref="R117" si="21">AD117/$AJ$8</f>
         <v>19.387117631565353</v>
       </c>
       <c r="S117" s="19">
-        <f t="shared" ref="S117" si="22">X117/$AC$8</f>
+        <f t="shared" ref="S117" si="22">AE117/$AJ$8</f>
         <v>22.91204811003178</v>
       </c>
       <c r="T117" s="20">
-        <f t="shared" ref="T117" si="23">Y117/$AC$8</f>
+        <f t="shared" ref="T117" si="23">AF117/$AJ$8</f>
         <v>24.674513349264995</v>
       </c>
-      <c r="V117">
+      <c r="U117" s="51"/>
+      <c r="V117" s="51"/>
+      <c r="W117" s="51"/>
+      <c r="X117" s="51"/>
+      <c r="Y117" s="51"/>
+      <c r="Z117" s="51"/>
+      <c r="AA117" s="51"/>
+      <c r="AC117">
         <f>20-8</f>
         <v>12</v>
       </c>
-      <c r="W117">
+      <c r="AD117">
         <f>18.5-7.5</f>
         <v>11</v>
       </c>
-      <c r="X117">
+      <c r="AE117">
         <f>22-9</f>
         <v>13</v>
       </c>
-      <c r="Y117">
+      <c r="AF117">
         <f>22-8</f>
         <v>14</v>
       </c>
     </row>
-    <row r="118" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:32" x14ac:dyDescent="0.3">
       <c r="E118">
         <v>2</v>
       </c>
@@ -4994,11 +5275,18 @@
       <c r="R118" s="21"/>
       <c r="S118" s="21"/>
       <c r="T118" s="22"/>
-      <c r="V118" s="2">
+      <c r="U118" s="52"/>
+      <c r="V118" s="52"/>
+      <c r="W118" s="52"/>
+      <c r="X118" s="52"/>
+      <c r="Y118" s="52"/>
+      <c r="Z118" s="52"/>
+      <c r="AA118" s="52"/>
+      <c r="AC118" s="2">
         <v>0.8</v>
       </c>
     </row>
-    <row r="119" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:32" x14ac:dyDescent="0.3">
       <c r="E119">
         <v>2</v>
       </c>
@@ -5024,39 +5312,46 @@
         <v>25</v>
       </c>
       <c r="Q119" s="19">
-        <f t="shared" ref="Q119" si="24">V119/$AC$8</f>
+        <f t="shared" ref="Q119" si="24">AC119/$AJ$8</f>
         <v>24.674513349264995</v>
       </c>
       <c r="R119" s="19">
-        <f t="shared" ref="R119" si="25">W119/$AC$8</f>
+        <f t="shared" ref="R119" si="25">AD119/$AJ$8</f>
         <v>24.674513349264995</v>
       </c>
       <c r="S119" s="19">
-        <f t="shared" ref="S119" si="26">X119/$AC$8</f>
+        <f t="shared" ref="S119" si="26">AE119/$AJ$8</f>
         <v>27.318211208114814</v>
       </c>
       <c r="T119" s="20">
-        <f t="shared" ref="T119" si="27">Y119/$AC$8</f>
+        <f t="shared" ref="T119" si="27">AF119/$AJ$8</f>
         <v>30.843141686581241</v>
       </c>
-      <c r="V119">
+      <c r="U119" s="51"/>
+      <c r="V119" s="51"/>
+      <c r="W119" s="51"/>
+      <c r="X119" s="51"/>
+      <c r="Y119" s="51"/>
+      <c r="Z119" s="51"/>
+      <c r="AA119" s="51"/>
+      <c r="AC119">
         <f>7.5+6.5</f>
         <v>14</v>
       </c>
-      <c r="W119">
+      <c r="AD119">
         <f>7.5+6.5</f>
         <v>14</v>
       </c>
-      <c r="X119">
+      <c r="AE119">
         <f>8+7.5</f>
         <v>15.5</v>
       </c>
-      <c r="Y119">
+      <c r="AF119">
         <f>8.5+9</f>
         <v>17.5</v>
       </c>
     </row>
-    <row r="120" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:32" x14ac:dyDescent="0.3">
       <c r="E120">
         <v>2</v>
       </c>
@@ -5082,39 +5377,46 @@
         <v>24.02</v>
       </c>
       <c r="Q120" s="19">
-        <f t="shared" ref="Q120:Q126" si="28">V120/$AC$8</f>
+        <f t="shared" ref="Q120:Q126" si="28">AC120/$AJ$8</f>
         <v>25.555745968881602</v>
       </c>
       <c r="R120" s="19">
-        <f t="shared" ref="R120" si="29">W120/$AC$8</f>
+        <f t="shared" ref="R120" si="29">AD120/$AJ$8</f>
         <v>23.793280729648387</v>
       </c>
       <c r="S120" s="19">
-        <f t="shared" ref="S120" si="30">X120/$AC$8</f>
+        <f t="shared" ref="S120" si="30">AE120/$AJ$8</f>
         <v>24.674513349264995</v>
       </c>
       <c r="T120" s="20">
-        <f t="shared" ref="T120" si="31">Y120/$AC$8</f>
+        <f t="shared" ref="T120" si="31">AF120/$AJ$8</f>
         <v>25.027006397111634</v>
       </c>
-      <c r="V120">
+      <c r="U120" s="51"/>
+      <c r="V120" s="51"/>
+      <c r="W120" s="51"/>
+      <c r="X120" s="51"/>
+      <c r="Y120" s="51"/>
+      <c r="Z120" s="51"/>
+      <c r="AA120" s="51"/>
+      <c r="AC120">
         <f>21-6.5</f>
         <v>14.5</v>
       </c>
-      <c r="W120">
+      <c r="AD120">
         <f>21-7.5</f>
         <v>13.5</v>
       </c>
-      <c r="X120">
+      <c r="AE120">
         <f>20.5-6.5</f>
         <v>14</v>
       </c>
-      <c r="Y120">
+      <c r="AF120">
         <f>21.2-7</f>
         <v>14.2</v>
       </c>
     </row>
-    <row r="121" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:32" x14ac:dyDescent="0.3">
       <c r="E121">
         <v>2</v>
       </c>
@@ -5126,11 +5428,18 @@
       <c r="R121" s="21"/>
       <c r="S121" s="21"/>
       <c r="T121" s="22"/>
-      <c r="V121" s="2">
+      <c r="U121" s="52"/>
+      <c r="V121" s="52"/>
+      <c r="W121" s="52"/>
+      <c r="X121" s="52"/>
+      <c r="Y121" s="52"/>
+      <c r="Z121" s="52"/>
+      <c r="AA121" s="52"/>
+      <c r="AC121" s="2">
         <v>0.8</v>
       </c>
     </row>
-    <row r="122" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:32" x14ac:dyDescent="0.3">
       <c r="E122">
         <v>2</v>
       </c>
@@ -5160,35 +5469,42 @@
         <v>27.318211208114814</v>
       </c>
       <c r="R122" s="19">
-        <f t="shared" ref="R122:R123" si="32">W122/$AC$8</f>
+        <f t="shared" ref="R122:R123" si="32">AD122/$AJ$8</f>
         <v>27.318211208114814</v>
       </c>
       <c r="S122" s="19">
-        <f t="shared" ref="S122:S123" si="33">X122/$AC$8</f>
+        <f t="shared" ref="S122:S123" si="33">AE122/$AJ$8</f>
         <v>27.318211208114814</v>
       </c>
       <c r="T122" s="20">
-        <f t="shared" ref="T122:T123" si="34">Y122/$AC$8</f>
+        <f t="shared" ref="T122:T123" si="34">AF122/$AJ$8</f>
         <v>28.199443827731422</v>
       </c>
-      <c r="V122">
+      <c r="U122" s="51"/>
+      <c r="V122" s="51"/>
+      <c r="W122" s="51"/>
+      <c r="X122" s="51"/>
+      <c r="Y122" s="51"/>
+      <c r="Z122" s="51"/>
+      <c r="AA122" s="51"/>
+      <c r="AC122">
         <f>9+6.5</f>
         <v>15.5</v>
       </c>
-      <c r="W122">
+      <c r="AD122">
         <f>9+6.5</f>
         <v>15.5</v>
       </c>
-      <c r="X122">
+      <c r="AE122">
         <f>9+6.5</f>
         <v>15.5</v>
       </c>
-      <c r="Y122">
+      <c r="AF122">
         <f>9.5+6.5</f>
         <v>16</v>
       </c>
     </row>
-    <row r="123" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:32" x14ac:dyDescent="0.3">
       <c r="E123">
         <v>2</v>
       </c>
@@ -5229,24 +5545,31 @@
         <f t="shared" si="34"/>
         <v>23.617034205725062</v>
       </c>
-      <c r="V123">
+      <c r="U123" s="51"/>
+      <c r="V123" s="51"/>
+      <c r="W123" s="51"/>
+      <c r="X123" s="51"/>
+      <c r="Y123" s="51"/>
+      <c r="Z123" s="51"/>
+      <c r="AA123" s="51"/>
+      <c r="AC123">
         <f>17.5-4</f>
         <v>13.5</v>
       </c>
-      <c r="W123">
+      <c r="AD123">
         <f>18-4.4</f>
         <v>13.6</v>
       </c>
-      <c r="X123">
+      <c r="AE123">
         <f>18.7-4.7</f>
         <v>14</v>
       </c>
-      <c r="Y123">
+      <c r="AF123">
         <f>19.2-5.8</f>
         <v>13.399999999999999</v>
       </c>
     </row>
-    <row r="124" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:32" x14ac:dyDescent="0.3">
       <c r="E124">
         <v>2</v>
       </c>
@@ -5255,11 +5578,11 @@
       </c>
       <c r="H124" s="11"/>
       <c r="Q124" s="21"/>
-      <c r="V124" s="2">
+      <c r="AC124" s="2">
         <v>0.8</v>
       </c>
     </row>
-    <row r="125" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:32" x14ac:dyDescent="0.3">
       <c r="E125">
         <v>2</v>
       </c>
@@ -5289,35 +5612,42 @@
         <v>27.318211208114814</v>
       </c>
       <c r="R125" s="19">
-        <f t="shared" ref="R125:R126" si="35">W125/$AC$8</f>
+        <f t="shared" ref="R125:R126" si="35">AD125/$AJ$8</f>
         <v>26.78947163634485</v>
       </c>
       <c r="S125" s="19">
-        <f t="shared" ref="S125:S126" si="36">X125/$AC$8</f>
+        <f t="shared" ref="S125:S126" si="36">AE125/$AJ$8</f>
         <v>28.199443827731422</v>
       </c>
       <c r="T125" s="20">
-        <f t="shared" ref="T125:T126" si="37">Y125/$AC$8</f>
+        <f t="shared" ref="T125:T126" si="37">AF125/$AJ$8</f>
         <v>25.555745968881602</v>
       </c>
-      <c r="V125">
+      <c r="U125" s="51"/>
+      <c r="V125" s="51"/>
+      <c r="W125" s="51"/>
+      <c r="X125" s="51"/>
+      <c r="Y125" s="51"/>
+      <c r="Z125" s="51"/>
+      <c r="AA125" s="51"/>
+      <c r="AC125">
         <f>9+6.5</f>
         <v>15.5</v>
       </c>
-      <c r="W125">
+      <c r="AD125">
         <f>9+6.2</f>
         <v>15.2</v>
       </c>
-      <c r="X125">
+      <c r="AE125">
         <f>9.5+6.5</f>
         <v>16</v>
       </c>
-      <c r="Y125">
+      <c r="AF125">
         <f>9+5.5</f>
         <v>14.5</v>
       </c>
     </row>
-    <row r="126" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:32" x14ac:dyDescent="0.3">
       <c r="E126">
         <v>2</v>
       </c>
@@ -5358,24 +5688,31 @@
         <f t="shared" si="37"/>
         <v>28.199443827731422</v>
       </c>
-      <c r="V126">
+      <c r="U126" s="51"/>
+      <c r="V126" s="51"/>
+      <c r="W126" s="51"/>
+      <c r="X126" s="51"/>
+      <c r="Y126" s="51"/>
+      <c r="Z126" s="51"/>
+      <c r="AA126" s="51"/>
+      <c r="AC126">
         <f>18-4.5</f>
         <v>13.5</v>
       </c>
-      <c r="W126">
+      <c r="AD126">
         <f>18-4.5</f>
         <v>13.5</v>
       </c>
-      <c r="X126">
+      <c r="AE126">
         <f>19-5</f>
         <v>14</v>
       </c>
-      <c r="Y126">
+      <c r="AF126">
         <f>23.5-7.5</f>
         <v>16</v>
       </c>
     </row>
-    <row r="127" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E127">
         <v>2</v>
       </c>
@@ -5383,7 +5720,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="128" spans="1:25" s="30" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:32" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A128" s="29" t="s">
         <v>42</v>
       </c>
@@ -6233,7 +6570,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="161" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:45" x14ac:dyDescent="0.3">
       <c r="H161" t="s">
         <v>59</v>
       </c>
@@ -6256,7 +6593,7 @@
         <v>17.283899999999999</v>
       </c>
     </row>
-    <row r="162" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:45" x14ac:dyDescent="0.3">
       <c r="G162" t="s">
         <v>4</v>
       </c>
@@ -6282,7 +6619,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="163" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:45" x14ac:dyDescent="0.3">
       <c r="H163" t="s">
         <v>32</v>
       </c>
@@ -6305,7 +6642,7 @@
         <v>21.5</v>
       </c>
     </row>
-    <row r="164" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:45" x14ac:dyDescent="0.3">
       <c r="H164" t="s">
         <v>59</v>
       </c>
@@ -6328,7 +6665,7 @@
         <v>2.9413999999999998</v>
       </c>
     </row>
-    <row r="165" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:45" x14ac:dyDescent="0.3">
       <c r="G165" t="s">
         <v>6</v>
       </c>
@@ -6354,7 +6691,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="166" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:45" x14ac:dyDescent="0.3">
       <c r="H166" t="s">
         <v>32</v>
       </c>
@@ -6377,7 +6714,7 @@
         <v>19.5</v>
       </c>
     </row>
-    <row r="167" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:45" x14ac:dyDescent="0.3">
       <c r="H167" t="s">
         <v>59</v>
       </c>
@@ -6400,7 +6737,7 @@
         <v>4.8673999999999999</v>
       </c>
     </row>
-    <row r="168" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>41</v>
       </c>
@@ -6444,7 +6781,7 @@
         <v>15.6</v>
       </c>
     </row>
-    <row r="169" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:45" x14ac:dyDescent="0.3">
       <c r="H169" t="s">
         <v>32</v>
       </c>
@@ -6467,7 +6804,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="170" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:45" x14ac:dyDescent="0.3">
       <c r="H170" t="s">
         <v>59</v>
       </c>
@@ -6490,8 +6827,15 @@
         <v>5.1585000000000001</v>
       </c>
       <c r="T170"/>
-    </row>
-    <row r="171" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="U170"/>
+      <c r="V170"/>
+      <c r="W170"/>
+      <c r="X170"/>
+      <c r="Y170"/>
+      <c r="Z170"/>
+      <c r="AA170"/>
+    </row>
+    <row r="171" spans="1:45" x14ac:dyDescent="0.3">
       <c r="G171" t="s">
         <v>5</v>
       </c>
@@ -6522,16 +6866,23 @@
       <c r="W171" s="14"/>
       <c r="X171" s="14"/>
       <c r="Y171" s="14"/>
+      <c r="Z171" s="14"/>
       <c r="AA171" s="14"/>
       <c r="AB171" s="14"/>
       <c r="AC171" s="14"/>
       <c r="AD171" s="14"/>
-      <c r="AG171" s="14"/>
+      <c r="AE171" s="14"/>
+      <c r="AF171" s="14"/>
       <c r="AH171" s="14"/>
+      <c r="AI171" s="14"/>
+      <c r="AJ171" s="14"/>
       <c r="AK171" s="14"/>
-      <c r="AL171" s="14"/>
-    </row>
-    <row r="172" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="AN171" s="14"/>
+      <c r="AO171" s="14"/>
+      <c r="AR171" s="14"/>
+      <c r="AS171" s="14"/>
+    </row>
+    <row r="172" spans="1:45" x14ac:dyDescent="0.3">
       <c r="H172" t="s">
         <v>32</v>
       </c>
@@ -6555,8 +6906,15 @@
       </c>
       <c r="R172" s="14"/>
       <c r="T172"/>
-    </row>
-    <row r="173" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="U172"/>
+      <c r="V172"/>
+      <c r="W172"/>
+      <c r="X172"/>
+      <c r="Y172"/>
+      <c r="Z172"/>
+      <c r="AA172"/>
+    </row>
+    <row r="173" spans="1:45" x14ac:dyDescent="0.3">
       <c r="H173" t="s">
         <v>59</v>
       </c>
@@ -6579,8 +6937,15 @@
         <v>18.452000000000002</v>
       </c>
       <c r="T173"/>
-    </row>
-    <row r="174" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="U173"/>
+      <c r="V173"/>
+      <c r="W173"/>
+      <c r="X173"/>
+      <c r="Y173"/>
+      <c r="Z173"/>
+      <c r="AA173"/>
+    </row>
+    <row r="174" spans="1:45" x14ac:dyDescent="0.3">
       <c r="G174" t="s">
         <v>4</v>
       </c>
@@ -6606,8 +6971,15 @@
         <v>10.5</v>
       </c>
       <c r="T174"/>
-    </row>
-    <row r="175" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="U174"/>
+      <c r="V174"/>
+      <c r="W174"/>
+      <c r="X174"/>
+      <c r="Y174"/>
+      <c r="Z174"/>
+      <c r="AA174"/>
+    </row>
+    <row r="175" spans="1:45" x14ac:dyDescent="0.3">
       <c r="H175" t="s">
         <v>32</v>
       </c>
@@ -6630,8 +7002,15 @@
         <v>16.5</v>
       </c>
       <c r="T175"/>
-    </row>
-    <row r="176" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="U175"/>
+      <c r="V175"/>
+      <c r="W175"/>
+      <c r="X175"/>
+      <c r="Y175"/>
+      <c r="Z175"/>
+      <c r="AA175"/>
+    </row>
+    <row r="176" spans="1:45" x14ac:dyDescent="0.3">
       <c r="H176" t="s">
         <v>59</v>
       </c>
@@ -6654,8 +7033,15 @@
         <v>2.6381999999999999</v>
       </c>
       <c r="T176"/>
-    </row>
-    <row r="177" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="U176"/>
+      <c r="V176"/>
+      <c r="W176"/>
+      <c r="X176"/>
+      <c r="Y176"/>
+      <c r="Z176"/>
+      <c r="AA176"/>
+    </row>
+    <row r="177" spans="1:35" x14ac:dyDescent="0.3">
       <c r="G177" t="s">
         <v>6</v>
       </c>
@@ -6681,9 +7067,16 @@
         <v>17</v>
       </c>
       <c r="T177"/>
-      <c r="AB177" s="14"/>
-    </row>
-    <row r="178" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="U177"/>
+      <c r="V177"/>
+      <c r="W177"/>
+      <c r="X177"/>
+      <c r="Y177"/>
+      <c r="Z177"/>
+      <c r="AA177"/>
+      <c r="AI177" s="14"/>
+    </row>
+    <row r="178" spans="1:35" x14ac:dyDescent="0.3">
       <c r="H178" t="s">
         <v>32</v>
       </c>
@@ -6706,9 +7099,16 @@
         <v>19.5</v>
       </c>
       <c r="T178"/>
-      <c r="AB178" s="14"/>
-    </row>
-    <row r="179" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="U178"/>
+      <c r="V178"/>
+      <c r="W178"/>
+      <c r="X178"/>
+      <c r="Y178"/>
+      <c r="Z178"/>
+      <c r="AA178"/>
+      <c r="AI178" s="14"/>
+    </row>
+    <row r="179" spans="1:35" x14ac:dyDescent="0.3">
       <c r="H179" t="s">
         <v>59</v>
       </c>
@@ -6731,7 +7131,7 @@
         <v>3.6564999999999999</v>
       </c>
     </row>
-    <row r="180" spans="1:28" s="41" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:35" s="41" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A180" s="41" t="s">
         <v>42</v>
       </c>
@@ -6767,9 +7167,16 @@
       <c r="X180" s="43"/>
       <c r="Y180" s="43"/>
       <c r="Z180" s="43"/>
+      <c r="AA180" s="43"/>
       <c r="AB180" s="43"/>
-    </row>
-    <row r="181" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="AC180" s="43"/>
+      <c r="AD180" s="43"/>
+      <c r="AE180" s="43"/>
+      <c r="AF180" s="43"/>
+      <c r="AG180" s="43"/>
+      <c r="AI180" s="43"/>
+    </row>
+    <row r="181" spans="1:35" x14ac:dyDescent="0.3">
       <c r="G181" s="14"/>
       <c r="H181" t="s">
         <v>32</v>
@@ -6785,9 +7192,16 @@
       </c>
       <c r="S181" s="14"/>
       <c r="T181"/>
-      <c r="AB181" s="14"/>
-    </row>
-    <row r="182" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="U181"/>
+      <c r="V181"/>
+      <c r="W181"/>
+      <c r="X181"/>
+      <c r="Y181"/>
+      <c r="Z181"/>
+      <c r="AA181"/>
+      <c r="AI181" s="14"/>
+    </row>
+    <row r="182" spans="1:35" x14ac:dyDescent="0.3">
       <c r="G182" s="14"/>
       <c r="H182" t="s">
         <v>59</v>
@@ -6812,10 +7226,17 @@
       </c>
       <c r="S182" s="14"/>
       <c r="T182"/>
-      <c r="AA182" s="14"/>
-      <c r="AB182" s="14"/>
-    </row>
-    <row r="183" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="U182"/>
+      <c r="V182"/>
+      <c r="W182"/>
+      <c r="X182"/>
+      <c r="Y182"/>
+      <c r="Z182"/>
+      <c r="AA182"/>
+      <c r="AH182" s="14"/>
+      <c r="AI182" s="14"/>
+    </row>
+    <row r="183" spans="1:35" x14ac:dyDescent="0.3">
       <c r="G183" s="14" t="s">
         <v>5</v>
       </c>
@@ -6842,8 +7263,15 @@
       </c>
       <c r="S183" s="14"/>
       <c r="T183"/>
-    </row>
-    <row r="184" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="U183"/>
+      <c r="V183"/>
+      <c r="W183"/>
+      <c r="X183"/>
+      <c r="Y183"/>
+      <c r="Z183"/>
+      <c r="AA183"/>
+    </row>
+    <row r="184" spans="1:35" x14ac:dyDescent="0.3">
       <c r="G184" s="14"/>
       <c r="H184" t="s">
         <v>32</v>
@@ -6868,9 +7296,16 @@
       </c>
       <c r="S184" s="14"/>
       <c r="T184"/>
-      <c r="AB184" s="14"/>
-    </row>
-    <row r="185" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="U184"/>
+      <c r="V184"/>
+      <c r="W184"/>
+      <c r="X184"/>
+      <c r="Y184"/>
+      <c r="Z184"/>
+      <c r="AA184"/>
+      <c r="AI184" s="14"/>
+    </row>
+    <row r="185" spans="1:35" x14ac:dyDescent="0.3">
       <c r="G185" s="14"/>
       <c r="H185" t="s">
         <v>59</v>
@@ -6894,110 +7329,298 @@
         <v>20</v>
       </c>
       <c r="T185"/>
-      <c r="AB185" s="14"/>
-    </row>
-    <row r="186" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="U185"/>
+      <c r="V185"/>
+      <c r="W185"/>
+      <c r="X185"/>
+      <c r="Y185"/>
+      <c r="Z185"/>
+      <c r="AA185"/>
+      <c r="AI185" s="14"/>
+    </row>
+    <row r="186" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="G186" t="s">
+        <v>3</v>
+      </c>
+      <c r="H186" t="s">
+        <v>61</v>
+      </c>
       <c r="I186"/>
       <c r="N186" s="13"/>
       <c r="S186" s="14"/>
       <c r="T186"/>
-      <c r="AB186" s="14"/>
-    </row>
-    <row r="187" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="U186">
+        <v>0.75529999999999997</v>
+      </c>
+      <c r="V186">
+        <v>0.75760000000000005</v>
+      </c>
+      <c r="W186">
+        <v>0.75219999999999998</v>
+      </c>
+      <c r="X186">
+        <v>0.73640000000000005</v>
+      </c>
+      <c r="Y186">
+        <v>0.74819999999999998</v>
+      </c>
+      <c r="Z186">
+        <v>0.72950000000000004</v>
+      </c>
+      <c r="AA186">
+        <v>0.70709999999999995</v>
+      </c>
+      <c r="AI186" s="14"/>
+    </row>
+    <row r="187" spans="1:35" x14ac:dyDescent="0.3">
       <c r="S187" s="14"/>
       <c r="T187"/>
-      <c r="Y187" s="14"/>
-      <c r="Z187" s="14"/>
-      <c r="AB187" s="14"/>
-    </row>
-    <row r="188" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="U187"/>
+      <c r="V187"/>
+      <c r="W187"/>
+      <c r="X187"/>
+      <c r="Y187"/>
+      <c r="Z187"/>
+      <c r="AA187"/>
+      <c r="AF187" s="14"/>
+      <c r="AG187" s="14"/>
+      <c r="AI187" s="14"/>
+    </row>
+    <row r="188" spans="1:35" x14ac:dyDescent="0.3">
       <c r="S188" s="14"/>
       <c r="T188"/>
-      <c r="AB188" s="14"/>
-    </row>
-    <row r="189" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="U188"/>
+      <c r="V188"/>
+      <c r="W188"/>
+      <c r="X188"/>
+      <c r="Y188"/>
+      <c r="Z188"/>
+      <c r="AA188"/>
+      <c r="AI188" s="14"/>
+    </row>
+    <row r="189" spans="1:35" x14ac:dyDescent="0.3">
       <c r="S189" s="14"/>
       <c r="T189"/>
-      <c r="AB189" s="14"/>
-    </row>
-    <row r="190" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="U189"/>
+      <c r="V189"/>
+      <c r="W189"/>
+      <c r="X189"/>
+      <c r="Y189"/>
+      <c r="Z189"/>
+      <c r="AA189"/>
+      <c r="AI189" s="14"/>
+    </row>
+    <row r="190" spans="1:35" x14ac:dyDescent="0.3">
       <c r="T190"/>
-      <c r="AB190" s="14"/>
-    </row>
-    <row r="191" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="U190"/>
+      <c r="V190"/>
+      <c r="W190"/>
+      <c r="X190"/>
+      <c r="Y190"/>
+      <c r="Z190"/>
+      <c r="AA190"/>
+      <c r="AI190" s="14"/>
+    </row>
+    <row r="191" spans="1:35" x14ac:dyDescent="0.3">
       <c r="T191"/>
-    </row>
-    <row r="192" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="U191"/>
+      <c r="V191"/>
+      <c r="W191"/>
+      <c r="X191"/>
+      <c r="Y191"/>
+      <c r="Z191"/>
+      <c r="AA191"/>
+    </row>
+    <row r="192" spans="1:35" x14ac:dyDescent="0.3">
       <c r="S192" s="14"/>
       <c r="T192"/>
-    </row>
-    <row r="193" spans="19:26" x14ac:dyDescent="0.3">
+      <c r="U192"/>
+      <c r="V192"/>
+      <c r="W192"/>
+      <c r="X192"/>
+      <c r="Y192"/>
+      <c r="Z192"/>
+      <c r="AA192"/>
+    </row>
+    <row r="193" spans="19:33" x14ac:dyDescent="0.3">
       <c r="S193" s="14"/>
       <c r="T193"/>
-    </row>
-    <row r="194" spans="19:26" x14ac:dyDescent="0.3">
+      <c r="U193"/>
+      <c r="V193"/>
+      <c r="W193"/>
+      <c r="X193"/>
+      <c r="Y193"/>
+      <c r="Z193"/>
+      <c r="AA193"/>
+    </row>
+    <row r="194" spans="19:33" x14ac:dyDescent="0.3">
       <c r="S194" s="14"/>
-      <c r="V194" s="14"/>
-      <c r="W194" s="14"/>
-      <c r="X194" s="14"/>
-      <c r="Y194" s="14"/>
-    </row>
-    <row r="195" spans="19:26" x14ac:dyDescent="0.3">
+      <c r="AC194" s="14"/>
+      <c r="AD194" s="14"/>
+      <c r="AE194" s="14"/>
+      <c r="AF194" s="14"/>
+    </row>
+    <row r="195" spans="19:33" x14ac:dyDescent="0.3">
       <c r="T195"/>
-    </row>
-    <row r="196" spans="19:26" x14ac:dyDescent="0.3">
+      <c r="U195"/>
+      <c r="V195"/>
+      <c r="W195"/>
+      <c r="X195"/>
+      <c r="Y195"/>
+      <c r="Z195"/>
+      <c r="AA195"/>
+    </row>
+    <row r="196" spans="19:33" x14ac:dyDescent="0.3">
       <c r="T196"/>
-    </row>
-    <row r="197" spans="19:26" x14ac:dyDescent="0.3">
+      <c r="U196"/>
+      <c r="V196"/>
+      <c r="W196"/>
+      <c r="X196"/>
+      <c r="Y196"/>
+      <c r="Z196"/>
+      <c r="AA196"/>
+    </row>
+    <row r="197" spans="19:33" x14ac:dyDescent="0.3">
       <c r="T197"/>
-    </row>
-    <row r="198" spans="19:26" x14ac:dyDescent="0.3">
+      <c r="U197"/>
+      <c r="V197"/>
+      <c r="W197"/>
+      <c r="X197"/>
+      <c r="Y197"/>
+      <c r="Z197"/>
+      <c r="AA197"/>
+    </row>
+    <row r="198" spans="19:33" x14ac:dyDescent="0.3">
       <c r="T198"/>
-    </row>
-    <row r="199" spans="19:26" x14ac:dyDescent="0.3">
+      <c r="U198"/>
+      <c r="V198"/>
+      <c r="W198"/>
+      <c r="X198"/>
+      <c r="Y198"/>
+      <c r="Z198"/>
+      <c r="AA198"/>
+    </row>
+    <row r="199" spans="19:33" x14ac:dyDescent="0.3">
       <c r="T199"/>
-    </row>
-    <row r="200" spans="19:26" x14ac:dyDescent="0.3">
+      <c r="U199"/>
+      <c r="V199"/>
+      <c r="W199"/>
+      <c r="X199"/>
+      <c r="Y199"/>
+      <c r="Z199"/>
+      <c r="AA199"/>
+    </row>
+    <row r="200" spans="19:33" x14ac:dyDescent="0.3">
       <c r="T200"/>
-      <c r="W200" s="14"/>
-    </row>
-    <row r="201" spans="19:26" x14ac:dyDescent="0.3">
+      <c r="U200"/>
+      <c r="V200"/>
+      <c r="W200"/>
+      <c r="X200"/>
+      <c r="Y200"/>
+      <c r="Z200"/>
+      <c r="AA200"/>
+      <c r="AD200" s="14"/>
+    </row>
+    <row r="201" spans="19:33" x14ac:dyDescent="0.3">
       <c r="T201"/>
-      <c r="W201" s="14"/>
-    </row>
-    <row r="202" spans="19:26" x14ac:dyDescent="0.3">
+      <c r="U201"/>
+      <c r="V201"/>
+      <c r="W201"/>
+      <c r="X201"/>
+      <c r="Y201"/>
+      <c r="Z201"/>
+      <c r="AA201"/>
+      <c r="AD201" s="14"/>
+    </row>
+    <row r="202" spans="19:33" x14ac:dyDescent="0.3">
       <c r="T202"/>
-    </row>
-    <row r="203" spans="19:26" x14ac:dyDescent="0.3">
+      <c r="U202"/>
+      <c r="V202"/>
+      <c r="W202"/>
+      <c r="X202"/>
+      <c r="Y202"/>
+      <c r="Z202"/>
+      <c r="AA202"/>
+    </row>
+    <row r="203" spans="19:33" x14ac:dyDescent="0.3">
       <c r="U203" s="14"/>
       <c r="V203" s="14"/>
       <c r="W203" s="14"/>
       <c r="X203" s="14"/>
       <c r="Y203" s="14"/>
       <c r="Z203" s="14"/>
-    </row>
-    <row r="204" spans="19:26" x14ac:dyDescent="0.3">
+      <c r="AA203" s="14"/>
+      <c r="AB203" s="14"/>
+      <c r="AC203" s="14"/>
+      <c r="AD203" s="14"/>
+      <c r="AE203" s="14"/>
+      <c r="AF203" s="14"/>
+      <c r="AG203" s="14"/>
+    </row>
+    <row r="204" spans="19:33" x14ac:dyDescent="0.3">
       <c r="T204"/>
-    </row>
-    <row r="205" spans="19:26" x14ac:dyDescent="0.3">
+      <c r="U204"/>
+      <c r="V204"/>
+      <c r="W204"/>
+      <c r="X204"/>
+      <c r="Y204"/>
+      <c r="Z204"/>
+      <c r="AA204"/>
+    </row>
+    <row r="205" spans="19:33" x14ac:dyDescent="0.3">
       <c r="T205"/>
-    </row>
-    <row r="206" spans="19:26" x14ac:dyDescent="0.3">
+      <c r="U205"/>
+      <c r="V205"/>
+      <c r="W205"/>
+      <c r="X205"/>
+      <c r="Y205"/>
+      <c r="Z205"/>
+      <c r="AA205"/>
+    </row>
+    <row r="206" spans="19:33" x14ac:dyDescent="0.3">
       <c r="T206"/>
-    </row>
-    <row r="207" spans="19:26" x14ac:dyDescent="0.3">
+      <c r="U206"/>
+      <c r="V206"/>
+      <c r="W206"/>
+      <c r="X206"/>
+      <c r="Y206"/>
+      <c r="Z206"/>
+      <c r="AA206"/>
+    </row>
+    <row r="207" spans="19:33" x14ac:dyDescent="0.3">
       <c r="T207"/>
-    </row>
-    <row r="208" spans="19:26" x14ac:dyDescent="0.3">
+      <c r="U207"/>
+      <c r="V207"/>
+      <c r="W207"/>
+      <c r="X207"/>
+      <c r="Y207"/>
+      <c r="Z207"/>
+      <c r="AA207"/>
+    </row>
+    <row r="208" spans="19:33" x14ac:dyDescent="0.3">
       <c r="T208"/>
-    </row>
-    <row r="209" spans="20:20" x14ac:dyDescent="0.3">
+      <c r="U208"/>
+      <c r="V208"/>
+      <c r="W208"/>
+      <c r="X208"/>
+      <c r="Y208"/>
+      <c r="Z208"/>
+      <c r="AA208"/>
+    </row>
+    <row r="209" spans="20:27" x14ac:dyDescent="0.3">
       <c r="T209"/>
+      <c r="U209"/>
+      <c r="V209"/>
+      <c r="W209"/>
+      <c r="X209"/>
+      <c r="Y209"/>
+      <c r="Z209"/>
+      <c r="AA209"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="AA2:AC2"/>
-    <mergeCell ref="W3:X3"/>
+    <mergeCell ref="AH2:AJ2"/>
+    <mergeCell ref="AD3:AE3"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
modified energy loss values given for 15 deg instead of 8
</commit_message>
<xml_diff>
--- a/cal/cal_results/CS_Ilena_Scattering_Results.xlsx
+++ b/cal/cal_results/CS_Ilena_Scattering_Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonny Woof\Google Drive\Python_packages_woof\pyMAP\cal\cal_results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA0BD6EF-317D-41BF-9BF4-5A3AA53654E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31E6E24A-DA59-4F80-90B4-943C087A439A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-11550" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cutfit fwhm" sheetId="3" r:id="rId1"/>
@@ -552,7 +552,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -597,6 +597,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -612,14 +614,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -902,8 +896,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:AS209"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F159" zoomScale="77" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="R187" sqref="R187"/>
+    <sheetView tabSelected="1" topLeftCell="A169" zoomScale="77" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F186" sqref="F186"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -913,16 +907,15 @@
     <col min="9" max="9" width="11.5546875" style="13"/>
     <col min="15" max="15" width="11.5546875" style="13"/>
     <col min="20" max="20" width="11.5546875" style="14"/>
-    <col min="21" max="27" width="11.5546875" style="49"/>
     <col min="28" max="28" width="24.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="AH2" s="44" t="s">
+      <c r="AH2" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="AI2" s="45"/>
-      <c r="AJ2" s="46"/>
+      <c r="AI2" s="47"/>
+      <c r="AJ2" s="48"/>
     </row>
     <row r="3" spans="1:36" x14ac:dyDescent="0.3">
       <c r="I3" s="13" t="s">
@@ -937,10 +930,10 @@
       <c r="Q3" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="AD3" s="47" t="s">
+      <c r="AD3" s="49" t="s">
         <v>26</v>
       </c>
-      <c r="AE3" s="48"/>
+      <c r="AE3" s="50"/>
       <c r="AH3" s="3" t="s">
         <v>14</v>
       </c>
@@ -1104,25 +1097,25 @@
         <f t="shared" si="0"/>
         <v>1000</v>
       </c>
-      <c r="U6" s="49">
+      <c r="U6">
         <v>14</v>
       </c>
-      <c r="V6" s="49">
+      <c r="V6">
         <v>27</v>
       </c>
-      <c r="W6" s="49">
+      <c r="W6">
         <v>52</v>
       </c>
-      <c r="X6" s="56">
+      <c r="X6">
         <v>102</v>
       </c>
-      <c r="Y6" s="56">
+      <c r="Y6">
         <v>197</v>
       </c>
-      <c r="Z6" s="56">
+      <c r="Z6">
         <v>451</v>
       </c>
-      <c r="AA6" s="56">
+      <c r="AA6">
         <v>908</v>
       </c>
       <c r="AD6" s="10" t="s">
@@ -1359,13 +1352,13 @@
       <c r="T10" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="U10" s="50"/>
-      <c r="V10" s="50"/>
-      <c r="W10" s="50"/>
-      <c r="X10" s="50"/>
-      <c r="Y10" s="50"/>
-      <c r="Z10" s="50"/>
-      <c r="AA10" s="50"/>
+      <c r="U10" s="17"/>
+      <c r="V10" s="17"/>
+      <c r="W10" s="17"/>
+      <c r="X10" s="17"/>
+      <c r="Y10" s="17"/>
+      <c r="Z10" s="17"/>
+      <c r="AA10" s="17"/>
       <c r="AC10">
         <f>10+8.5</f>
         <v>18.5</v>
@@ -1634,13 +1627,13 @@
       <c r="T16" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="U16" s="50"/>
-      <c r="V16" s="50"/>
-      <c r="W16" s="50"/>
-      <c r="X16" s="50"/>
-      <c r="Y16" s="50"/>
-      <c r="Z16" s="50"/>
-      <c r="AA16" s="50"/>
+      <c r="U16" s="17"/>
+      <c r="V16" s="17"/>
+      <c r="W16" s="17"/>
+      <c r="X16" s="17"/>
+      <c r="Y16" s="17"/>
+      <c r="Z16" s="17"/>
+      <c r="AA16" s="17"/>
       <c r="AC16">
         <f>9+8.5</f>
         <v>17.5</v>
@@ -1972,13 +1965,13 @@
         <v>17.2</v>
       </c>
       <c r="T26" s="18"/>
-      <c r="U26" s="50"/>
-      <c r="V26" s="50"/>
-      <c r="W26" s="50"/>
-      <c r="X26" s="50"/>
-      <c r="Y26" s="50"/>
-      <c r="Z26" s="50"/>
-      <c r="AA26" s="50"/>
+      <c r="U26" s="17"/>
+      <c r="V26" s="17"/>
+      <c r="W26" s="17"/>
+      <c r="X26" s="17"/>
+      <c r="Y26" s="17"/>
+      <c r="Z26" s="17"/>
+      <c r="AA26" s="17"/>
       <c r="AD26" t="s">
         <v>20</v>
       </c>
@@ -2196,13 +2189,13 @@
         <f>AF33/$AJ$8</f>
         <v>27.494457732038136</v>
       </c>
-      <c r="U33" s="51"/>
-      <c r="V33" s="51"/>
-      <c r="W33" s="51"/>
-      <c r="X33" s="51"/>
-      <c r="Y33" s="51"/>
-      <c r="Z33" s="51"/>
-      <c r="AA33" s="51"/>
+      <c r="U33" s="19"/>
+      <c r="V33" s="19"/>
+      <c r="W33" s="19"/>
+      <c r="X33" s="19"/>
+      <c r="Y33" s="19"/>
+      <c r="Z33" s="19"/>
+      <c r="AA33" s="19"/>
       <c r="AC33">
         <f>9+7.5</f>
         <v>16.5</v>
@@ -2259,13 +2252,13 @@
         <f>AF34/$AJ$8</f>
         <v>21.502075918645211</v>
       </c>
-      <c r="U34" s="51"/>
-      <c r="V34" s="51"/>
-      <c r="W34" s="51"/>
-      <c r="X34" s="51"/>
-      <c r="Y34" s="51"/>
-      <c r="Z34" s="51"/>
-      <c r="AA34" s="51"/>
+      <c r="U34" s="19"/>
+      <c r="V34" s="19"/>
+      <c r="W34" s="19"/>
+      <c r="X34" s="19"/>
+      <c r="Y34" s="19"/>
+      <c r="Z34" s="19"/>
+      <c r="AA34" s="19"/>
       <c r="AC34">
         <f>19.5-5.8</f>
         <v>13.7</v>
@@ -2294,13 +2287,13 @@
       <c r="R35" s="21"/>
       <c r="S35" s="21"/>
       <c r="T35" s="22"/>
-      <c r="U35" s="52"/>
-      <c r="V35" s="52"/>
-      <c r="W35" s="52"/>
-      <c r="X35" s="52"/>
-      <c r="Y35" s="52"/>
-      <c r="Z35" s="52"/>
-      <c r="AA35" s="52"/>
+      <c r="U35" s="21"/>
+      <c r="V35" s="21"/>
+      <c r="W35" s="21"/>
+      <c r="X35" s="21"/>
+      <c r="Y35" s="21"/>
+      <c r="Z35" s="21"/>
+      <c r="AA35" s="21"/>
     </row>
     <row r="36" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A36" s="13"/>
@@ -2341,13 +2334,13 @@
         <f t="shared" si="5"/>
         <v>28.551936875578065</v>
       </c>
-      <c r="U36" s="51"/>
-      <c r="V36" s="51"/>
-      <c r="W36" s="51"/>
-      <c r="X36" s="51"/>
-      <c r="Y36" s="51"/>
-      <c r="Z36" s="51"/>
-      <c r="AA36" s="51"/>
+      <c r="U36" s="19"/>
+      <c r="V36" s="19"/>
+      <c r="W36" s="19"/>
+      <c r="X36" s="19"/>
+      <c r="Y36" s="19"/>
+      <c r="Z36" s="19"/>
+      <c r="AA36" s="19"/>
       <c r="AC36">
         <f>7+7.2</f>
         <v>14.2</v>
@@ -2407,13 +2400,13 @@
         <f t="shared" ref="T37" si="8">AF37/$AJ$8</f>
         <v>22.91204811003178</v>
       </c>
-      <c r="U37" s="51"/>
-      <c r="V37" s="51"/>
-      <c r="W37" s="51"/>
-      <c r="X37" s="51"/>
-      <c r="Y37" s="51"/>
-      <c r="Z37" s="51"/>
-      <c r="AA37" s="51"/>
+      <c r="U37" s="19"/>
+      <c r="V37" s="19"/>
+      <c r="W37" s="19"/>
+      <c r="X37" s="19"/>
+      <c r="Y37" s="19"/>
+      <c r="Z37" s="19"/>
+      <c r="AA37" s="19"/>
       <c r="AC37">
         <f>19.2-7</f>
         <v>12.2</v>
@@ -2441,13 +2434,13 @@
       <c r="R38" s="21"/>
       <c r="S38" s="21"/>
       <c r="T38" s="22"/>
-      <c r="U38" s="52"/>
-      <c r="V38" s="52"/>
-      <c r="W38" s="52"/>
-      <c r="X38" s="52"/>
-      <c r="Y38" s="52"/>
-      <c r="Z38" s="52"/>
-      <c r="AA38" s="52"/>
+      <c r="U38" s="21"/>
+      <c r="V38" s="21"/>
+      <c r="W38" s="21"/>
+      <c r="X38" s="21"/>
+      <c r="Y38" s="21"/>
+      <c r="Z38" s="21"/>
+      <c r="AA38" s="21"/>
     </row>
     <row r="39" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A39" s="13"/>
@@ -2488,13 +2481,13 @@
         <f t="shared" si="9"/>
         <v>24.395767087225131</v>
       </c>
-      <c r="U39" s="51"/>
-      <c r="V39" s="51"/>
-      <c r="W39" s="51"/>
-      <c r="X39" s="51"/>
-      <c r="Y39" s="51"/>
-      <c r="Z39" s="51"/>
-      <c r="AA39" s="51"/>
+      <c r="U39" s="19"/>
+      <c r="V39" s="19"/>
+      <c r="W39" s="19"/>
+      <c r="X39" s="19"/>
+      <c r="Y39" s="19"/>
+      <c r="Z39" s="19"/>
+      <c r="AA39" s="19"/>
       <c r="AC39">
         <f>9.5+6.5</f>
         <v>16</v>
@@ -2554,13 +2547,13 @@
         <f t="shared" ref="T40" si="12">AF40/$AJ$7</f>
         <v>24.116958320513987</v>
       </c>
-      <c r="U40" s="51"/>
-      <c r="V40" s="51"/>
-      <c r="W40" s="51"/>
-      <c r="X40" s="51"/>
-      <c r="Y40" s="51"/>
-      <c r="Z40" s="51"/>
-      <c r="AA40" s="51"/>
+      <c r="U40" s="19"/>
+      <c r="V40" s="19"/>
+      <c r="W40" s="19"/>
+      <c r="X40" s="19"/>
+      <c r="Y40" s="19"/>
+      <c r="Z40" s="19"/>
+      <c r="AA40" s="19"/>
       <c r="AC40">
         <f>21-5.5</f>
         <v>15.5</v>
@@ -2588,13 +2581,13 @@
       <c r="R41" s="21"/>
       <c r="S41" s="21"/>
       <c r="T41" s="22"/>
-      <c r="U41" s="52"/>
-      <c r="V41" s="52"/>
-      <c r="W41" s="52"/>
-      <c r="X41" s="52"/>
-      <c r="Y41" s="52"/>
-      <c r="Z41" s="52"/>
-      <c r="AA41" s="52"/>
+      <c r="U41" s="21"/>
+      <c r="V41" s="21"/>
+      <c r="W41" s="21"/>
+      <c r="X41" s="21"/>
+      <c r="Y41" s="21"/>
+      <c r="Z41" s="21"/>
+      <c r="AA41" s="21"/>
       <c r="AC41" s="2">
         <v>0.7</v>
       </c>
@@ -2641,13 +2634,13 @@
         <f>AF42/$AJ$8</f>
         <v>25.203252921034959</v>
       </c>
-      <c r="U42" s="51"/>
-      <c r="V42" s="51"/>
-      <c r="W42" s="51"/>
-      <c r="X42" s="51"/>
-      <c r="Y42" s="51"/>
-      <c r="Z42" s="51"/>
-      <c r="AA42" s="51"/>
+      <c r="U42" s="19"/>
+      <c r="V42" s="19"/>
+      <c r="W42" s="19"/>
+      <c r="X42" s="19"/>
+      <c r="Y42" s="19"/>
+      <c r="Z42" s="19"/>
+      <c r="AA42" s="19"/>
       <c r="AC42">
         <f>17</f>
         <v>17</v>
@@ -2704,13 +2697,13 @@
         <f>AF43/$AJ$8</f>
         <v>22.383308538261815</v>
       </c>
-      <c r="U43" s="51"/>
-      <c r="V43" s="51"/>
-      <c r="W43" s="51"/>
-      <c r="X43" s="51"/>
-      <c r="Y43" s="51"/>
-      <c r="Z43" s="51"/>
-      <c r="AA43" s="51"/>
+      <c r="U43" s="19"/>
+      <c r="V43" s="19"/>
+      <c r="W43" s="19"/>
+      <c r="X43" s="19"/>
+      <c r="Y43" s="19"/>
+      <c r="Z43" s="19"/>
+      <c r="AA43" s="19"/>
       <c r="AC43">
         <f>20.5-5.5</f>
         <v>15</v>
@@ -2827,13 +2820,13 @@
         <f>AF47/$AJ$6</f>
         <v>21.200581908978378</v>
       </c>
-      <c r="U47" s="50"/>
-      <c r="V47" s="50"/>
-      <c r="W47" s="50"/>
-      <c r="X47" s="50"/>
-      <c r="Y47" s="50"/>
-      <c r="Z47" s="50"/>
-      <c r="AA47" s="50"/>
+      <c r="U47" s="17"/>
+      <c r="V47" s="17"/>
+      <c r="W47" s="17"/>
+      <c r="X47" s="17"/>
+      <c r="Y47" s="17"/>
+      <c r="Z47" s="17"/>
+      <c r="AA47" s="17"/>
       <c r="AE47">
         <f>20.7-3.3</f>
         <v>17.399999999999999</v>
@@ -2899,13 +2892,13 @@
         <f>AF48/$AJ$6</f>
         <v>20.851121767621596</v>
       </c>
-      <c r="U48" s="50"/>
-      <c r="V48" s="50"/>
-      <c r="W48" s="50"/>
-      <c r="X48" s="50"/>
-      <c r="Y48" s="50"/>
-      <c r="Z48" s="50"/>
-      <c r="AA48" s="50"/>
+      <c r="U48" s="17"/>
+      <c r="V48" s="17"/>
+      <c r="W48" s="17"/>
+      <c r="X48" s="17"/>
+      <c r="Y48" s="17"/>
+      <c r="Z48" s="17"/>
+      <c r="AA48" s="17"/>
       <c r="AE48">
         <f>20.5-3.3</f>
         <v>17.2</v>
@@ -3056,13 +3049,13 @@
         <f>AF53/$AJ$7</f>
         <v>17.146739152735378</v>
       </c>
-      <c r="U53" s="50"/>
-      <c r="V53" s="50"/>
-      <c r="W53" s="50"/>
-      <c r="X53" s="50"/>
-      <c r="Y53" s="50"/>
-      <c r="Z53" s="50"/>
-      <c r="AA53" s="50"/>
+      <c r="U53" s="17"/>
+      <c r="V53" s="17"/>
+      <c r="W53" s="17"/>
+      <c r="X53" s="17"/>
+      <c r="Y53" s="17"/>
+      <c r="Z53" s="17"/>
+      <c r="AA53" s="17"/>
       <c r="AC53">
         <f>8+5.5</f>
         <v>13.5</v>
@@ -3122,13 +3115,13 @@
         <f>AF54/$AJ$7</f>
         <v>20.631848736624683</v>
       </c>
-      <c r="U54" s="50"/>
-      <c r="V54" s="50"/>
-      <c r="W54" s="50"/>
-      <c r="X54" s="50"/>
-      <c r="Y54" s="50"/>
-      <c r="Z54" s="50"/>
-      <c r="AA54" s="50"/>
+      <c r="U54" s="17"/>
+      <c r="V54" s="17"/>
+      <c r="W54" s="17"/>
+      <c r="X54" s="17"/>
+      <c r="Y54" s="17"/>
+      <c r="Z54" s="17"/>
+      <c r="AA54" s="17"/>
       <c r="AC54">
         <f>20-3</f>
         <v>17</v>
@@ -3207,13 +3200,13 @@
         <f t="shared" si="15"/>
         <v>21.328870653402543</v>
       </c>
-      <c r="U56" s="50"/>
-      <c r="V56" s="50"/>
-      <c r="W56" s="50"/>
-      <c r="X56" s="50"/>
-      <c r="Y56" s="50"/>
-      <c r="Z56" s="50"/>
-      <c r="AA56" s="50"/>
+      <c r="U56" s="17"/>
+      <c r="V56" s="17"/>
+      <c r="W56" s="17"/>
+      <c r="X56" s="17"/>
+      <c r="Y56" s="17"/>
+      <c r="Z56" s="17"/>
+      <c r="AA56" s="17"/>
       <c r="AC56">
         <f>7.5+6.4</f>
         <v>13.9</v>
@@ -3273,13 +3266,13 @@
         <f t="shared" si="15"/>
         <v>26.486832837558712</v>
       </c>
-      <c r="U57" s="50"/>
-      <c r="V57" s="50"/>
-      <c r="W57" s="50"/>
-      <c r="X57" s="50"/>
-      <c r="Y57" s="50"/>
-      <c r="Z57" s="50"/>
-      <c r="AA57" s="50"/>
+      <c r="U57" s="17"/>
+      <c r="V57" s="17"/>
+      <c r="W57" s="17"/>
+      <c r="X57" s="17"/>
+      <c r="Y57" s="17"/>
+      <c r="Z57" s="17"/>
+      <c r="AA57" s="17"/>
       <c r="AC57">
         <f>19.2-3.2</f>
         <v>16</v>
@@ -3381,13 +3374,13 @@
         <f>AF61/AJ7</f>
         <v>19.934826819846823</v>
       </c>
-      <c r="U61" s="50"/>
-      <c r="V61" s="50"/>
-      <c r="W61" s="50"/>
-      <c r="X61" s="50"/>
-      <c r="Y61" s="50"/>
-      <c r="Z61" s="50"/>
-      <c r="AA61" s="50"/>
+      <c r="U61" s="17"/>
+      <c r="V61" s="17"/>
+      <c r="W61" s="17"/>
+      <c r="X61" s="17"/>
+      <c r="Y61" s="17"/>
+      <c r="Z61" s="17"/>
+      <c r="AA61" s="17"/>
       <c r="AE61">
         <f>20.3-1.8</f>
         <v>18.5</v>
@@ -3447,13 +3440,13 @@
         <f>AF62/AJ7</f>
         <v>21.468275036758115</v>
       </c>
-      <c r="U62" s="50"/>
-      <c r="V62" s="50"/>
-      <c r="W62" s="50"/>
-      <c r="X62" s="50"/>
-      <c r="Y62" s="50"/>
-      <c r="Z62" s="50"/>
-      <c r="AA62" s="50"/>
+      <c r="U62" s="17"/>
+      <c r="V62" s="17"/>
+      <c r="W62" s="17"/>
+      <c r="X62" s="17"/>
+      <c r="Y62" s="17"/>
+      <c r="Z62" s="17"/>
+      <c r="AA62" s="17"/>
       <c r="AE62">
         <f>9+8.4</f>
         <v>17.399999999999999</v>
@@ -3527,13 +3520,13 @@
         <f t="shared" si="16"/>
         <v>24.116958320513987</v>
       </c>
-      <c r="U64" s="50"/>
-      <c r="V64" s="50"/>
-      <c r="W64" s="50"/>
-      <c r="X64" s="50"/>
-      <c r="Y64" s="50"/>
-      <c r="Z64" s="50"/>
-      <c r="AA64" s="50"/>
+      <c r="U64" s="17"/>
+      <c r="V64" s="17"/>
+      <c r="W64" s="17"/>
+      <c r="X64" s="17"/>
+      <c r="Y64" s="17"/>
+      <c r="Z64" s="17"/>
+      <c r="AA64" s="17"/>
       <c r="AC64">
         <f>6.5+6.7</f>
         <v>13.2</v>
@@ -3605,13 +3598,13 @@
         <f t="shared" ref="T65" si="19">AG65/$AJ$7</f>
         <v>18.680187369646667</v>
       </c>
-      <c r="U65" s="50"/>
-      <c r="V65" s="50"/>
-      <c r="W65" s="50"/>
-      <c r="X65" s="50"/>
-      <c r="Y65" s="50"/>
-      <c r="Z65" s="50"/>
-      <c r="AA65" s="50"/>
+      <c r="U65" s="17"/>
+      <c r="V65" s="17"/>
+      <c r="W65" s="17"/>
+      <c r="X65" s="17"/>
+      <c r="Y65" s="17"/>
+      <c r="Z65" s="17"/>
+      <c r="AA65" s="17"/>
       <c r="AC65">
         <f>19-2</f>
         <v>17</v>
@@ -3685,13 +3678,13 @@
         <f>AF67/$AJ$6</f>
         <v>16.657600071340156</v>
       </c>
-      <c r="U67" s="50"/>
-      <c r="V67" s="50"/>
-      <c r="W67" s="50"/>
-      <c r="X67" s="50"/>
-      <c r="Y67" s="50"/>
-      <c r="Z67" s="50"/>
-      <c r="AA67" s="50"/>
+      <c r="U67" s="17"/>
+      <c r="V67" s="17"/>
+      <c r="W67" s="17"/>
+      <c r="X67" s="17"/>
+      <c r="Y67" s="17"/>
+      <c r="Z67" s="17"/>
+      <c r="AA67" s="17"/>
       <c r="AD67" t="s">
         <v>24</v>
       </c>
@@ -3746,13 +3739,13 @@
         <f>AF68/$AJ$6</f>
         <v>21.666528764120759</v>
       </c>
-      <c r="U68" s="50"/>
-      <c r="V68" s="50"/>
-      <c r="W68" s="50"/>
-      <c r="X68" s="50"/>
-      <c r="Y68" s="50"/>
-      <c r="Z68" s="50"/>
-      <c r="AA68" s="50"/>
+      <c r="U68" s="17"/>
+      <c r="V68" s="17"/>
+      <c r="W68" s="17"/>
+      <c r="X68" s="17"/>
+      <c r="Y68" s="17"/>
+      <c r="Z68" s="17"/>
+      <c r="AA68" s="17"/>
       <c r="AE68">
         <f>17.7-1.5</f>
         <v>16.2</v>
@@ -3814,13 +3807,13 @@
       <c r="R70" s="25"/>
       <c r="S70" s="25"/>
       <c r="T70" s="26"/>
-      <c r="U70" s="53"/>
-      <c r="V70" s="53"/>
-      <c r="W70" s="53"/>
-      <c r="X70" s="53"/>
-      <c r="Y70" s="53"/>
-      <c r="Z70" s="53"/>
-      <c r="AA70" s="53"/>
+      <c r="U70" s="25"/>
+      <c r="V70" s="25"/>
+      <c r="W70" s="25"/>
+      <c r="X70" s="25"/>
+      <c r="Y70" s="25"/>
+      <c r="Z70" s="25"/>
+      <c r="AA70" s="25"/>
       <c r="AC70">
         <f>7.3+5.5</f>
         <v>12.8</v>
@@ -3880,13 +3873,13 @@
         <f>AF71/$AJ$8</f>
         <v>26.436978588498206</v>
       </c>
-      <c r="U71" s="50"/>
-      <c r="V71" s="50"/>
-      <c r="W71" s="50"/>
-      <c r="X71" s="50"/>
-      <c r="Y71" s="50"/>
-      <c r="Z71" s="50"/>
-      <c r="AA71" s="50"/>
+      <c r="U71" s="17"/>
+      <c r="V71" s="17"/>
+      <c r="W71" s="17"/>
+      <c r="X71" s="17"/>
+      <c r="Y71" s="17"/>
+      <c r="Z71" s="17"/>
+      <c r="AA71" s="17"/>
       <c r="AC71">
         <f>17-1.4</f>
         <v>15.6</v>
@@ -4695,13 +4688,13 @@
         <f>18.7-1.7</f>
         <v>17</v>
       </c>
-      <c r="U98" s="54"/>
-      <c r="V98" s="54"/>
-      <c r="W98" s="54"/>
-      <c r="X98" s="54"/>
-      <c r="Y98" s="54"/>
-      <c r="Z98" s="54"/>
-      <c r="AA98" s="54"/>
+      <c r="U98" s="44"/>
+      <c r="V98" s="44"/>
+      <c r="W98" s="44"/>
+      <c r="X98" s="44"/>
+      <c r="Y98" s="44"/>
+      <c r="Z98" s="44"/>
+      <c r="AA98" s="44"/>
     </row>
     <row r="99" spans="5:30" x14ac:dyDescent="0.3">
       <c r="E99">
@@ -4865,13 +4858,13 @@
         <f>AD105/AJ6</f>
         <v>21.666528764120763</v>
       </c>
-      <c r="U105" s="55"/>
-      <c r="V105" s="55"/>
-      <c r="W105" s="55"/>
-      <c r="X105" s="55"/>
-      <c r="Y105" s="55"/>
-      <c r="Z105" s="55"/>
-      <c r="AA105" s="55"/>
+      <c r="U105" s="45"/>
+      <c r="V105" s="45"/>
+      <c r="W105" s="45"/>
+      <c r="X105" s="45"/>
+      <c r="Y105" s="45"/>
+      <c r="Z105" s="45"/>
+      <c r="AA105" s="45"/>
       <c r="AD105">
         <f>8+10.6</f>
         <v>18.600000000000001</v>
@@ -5173,13 +5166,13 @@
         <f t="shared" si="20"/>
         <v>23.969527253571709</v>
       </c>
-      <c r="U116" s="51"/>
-      <c r="V116" s="51"/>
-      <c r="W116" s="51"/>
-      <c r="X116" s="51"/>
-      <c r="Y116" s="51"/>
-      <c r="Z116" s="51"/>
-      <c r="AA116" s="51"/>
+      <c r="U116" s="19"/>
+      <c r="V116" s="19"/>
+      <c r="W116" s="19"/>
+      <c r="X116" s="19"/>
+      <c r="Y116" s="19"/>
+      <c r="Z116" s="19"/>
+      <c r="AA116" s="19"/>
       <c r="AC116">
         <f>7+4</f>
         <v>11</v>
@@ -5238,13 +5231,13 @@
         <f t="shared" ref="T117" si="23">AF117/$AJ$8</f>
         <v>24.674513349264995</v>
       </c>
-      <c r="U117" s="51"/>
-      <c r="V117" s="51"/>
-      <c r="W117" s="51"/>
-      <c r="X117" s="51"/>
-      <c r="Y117" s="51"/>
-      <c r="Z117" s="51"/>
-      <c r="AA117" s="51"/>
+      <c r="U117" s="19"/>
+      <c r="V117" s="19"/>
+      <c r="W117" s="19"/>
+      <c r="X117" s="19"/>
+      <c r="Y117" s="19"/>
+      <c r="Z117" s="19"/>
+      <c r="AA117" s="19"/>
       <c r="AC117">
         <f>20-8</f>
         <v>12</v>
@@ -5275,13 +5268,13 @@
       <c r="R118" s="21"/>
       <c r="S118" s="21"/>
       <c r="T118" s="22"/>
-      <c r="U118" s="52"/>
-      <c r="V118" s="52"/>
-      <c r="W118" s="52"/>
-      <c r="X118" s="52"/>
-      <c r="Y118" s="52"/>
-      <c r="Z118" s="52"/>
-      <c r="AA118" s="52"/>
+      <c r="U118" s="21"/>
+      <c r="V118" s="21"/>
+      <c r="W118" s="21"/>
+      <c r="X118" s="21"/>
+      <c r="Y118" s="21"/>
+      <c r="Z118" s="21"/>
+      <c r="AA118" s="21"/>
       <c r="AC118" s="2">
         <v>0.8</v>
       </c>
@@ -5327,13 +5320,13 @@
         <f t="shared" ref="T119" si="27">AF119/$AJ$8</f>
         <v>30.843141686581241</v>
       </c>
-      <c r="U119" s="51"/>
-      <c r="V119" s="51"/>
-      <c r="W119" s="51"/>
-      <c r="X119" s="51"/>
-      <c r="Y119" s="51"/>
-      <c r="Z119" s="51"/>
-      <c r="AA119" s="51"/>
+      <c r="U119" s="19"/>
+      <c r="V119" s="19"/>
+      <c r="W119" s="19"/>
+      <c r="X119" s="19"/>
+      <c r="Y119" s="19"/>
+      <c r="Z119" s="19"/>
+      <c r="AA119" s="19"/>
       <c r="AC119">
         <f>7.5+6.5</f>
         <v>14</v>
@@ -5392,13 +5385,13 @@
         <f t="shared" ref="T120" si="31">AF120/$AJ$8</f>
         <v>25.027006397111634</v>
       </c>
-      <c r="U120" s="51"/>
-      <c r="V120" s="51"/>
-      <c r="W120" s="51"/>
-      <c r="X120" s="51"/>
-      <c r="Y120" s="51"/>
-      <c r="Z120" s="51"/>
-      <c r="AA120" s="51"/>
+      <c r="U120" s="19"/>
+      <c r="V120" s="19"/>
+      <c r="W120" s="19"/>
+      <c r="X120" s="19"/>
+      <c r="Y120" s="19"/>
+      <c r="Z120" s="19"/>
+      <c r="AA120" s="19"/>
       <c r="AC120">
         <f>21-6.5</f>
         <v>14.5</v>
@@ -5428,13 +5421,13 @@
       <c r="R121" s="21"/>
       <c r="S121" s="21"/>
       <c r="T121" s="22"/>
-      <c r="U121" s="52"/>
-      <c r="V121" s="52"/>
-      <c r="W121" s="52"/>
-      <c r="X121" s="52"/>
-      <c r="Y121" s="52"/>
-      <c r="Z121" s="52"/>
-      <c r="AA121" s="52"/>
+      <c r="U121" s="21"/>
+      <c r="V121" s="21"/>
+      <c r="W121" s="21"/>
+      <c r="X121" s="21"/>
+      <c r="Y121" s="21"/>
+      <c r="Z121" s="21"/>
+      <c r="AA121" s="21"/>
       <c r="AC121" s="2">
         <v>0.8</v>
       </c>
@@ -5480,13 +5473,13 @@
         <f t="shared" ref="T122:T123" si="34">AF122/$AJ$8</f>
         <v>28.199443827731422</v>
       </c>
-      <c r="U122" s="51"/>
-      <c r="V122" s="51"/>
-      <c r="W122" s="51"/>
-      <c r="X122" s="51"/>
-      <c r="Y122" s="51"/>
-      <c r="Z122" s="51"/>
-      <c r="AA122" s="51"/>
+      <c r="U122" s="19"/>
+      <c r="V122" s="19"/>
+      <c r="W122" s="19"/>
+      <c r="X122" s="19"/>
+      <c r="Y122" s="19"/>
+      <c r="Z122" s="19"/>
+      <c r="AA122" s="19"/>
       <c r="AC122">
         <f>9+6.5</f>
         <v>15.5</v>
@@ -5545,13 +5538,13 @@
         <f t="shared" si="34"/>
         <v>23.617034205725062</v>
       </c>
-      <c r="U123" s="51"/>
-      <c r="V123" s="51"/>
-      <c r="W123" s="51"/>
-      <c r="X123" s="51"/>
-      <c r="Y123" s="51"/>
-      <c r="Z123" s="51"/>
-      <c r="AA123" s="51"/>
+      <c r="U123" s="19"/>
+      <c r="V123" s="19"/>
+      <c r="W123" s="19"/>
+      <c r="X123" s="19"/>
+      <c r="Y123" s="19"/>
+      <c r="Z123" s="19"/>
+      <c r="AA123" s="19"/>
       <c r="AC123">
         <f>17.5-4</f>
         <v>13.5</v>
@@ -5623,13 +5616,13 @@
         <f t="shared" ref="T125:T126" si="37">AF125/$AJ$8</f>
         <v>25.555745968881602</v>
       </c>
-      <c r="U125" s="51"/>
-      <c r="V125" s="51"/>
-      <c r="W125" s="51"/>
-      <c r="X125" s="51"/>
-      <c r="Y125" s="51"/>
-      <c r="Z125" s="51"/>
-      <c r="AA125" s="51"/>
+      <c r="U125" s="19"/>
+      <c r="V125" s="19"/>
+      <c r="W125" s="19"/>
+      <c r="X125" s="19"/>
+      <c r="Y125" s="19"/>
+      <c r="Z125" s="19"/>
+      <c r="AA125" s="19"/>
       <c r="AC125">
         <f>9+6.5</f>
         <v>15.5</v>
@@ -5688,13 +5681,13 @@
         <f t="shared" si="37"/>
         <v>28.199443827731422</v>
       </c>
-      <c r="U126" s="51"/>
-      <c r="V126" s="51"/>
-      <c r="W126" s="51"/>
-      <c r="X126" s="51"/>
-      <c r="Y126" s="51"/>
-      <c r="Z126" s="51"/>
-      <c r="AA126" s="51"/>
+      <c r="U126" s="19"/>
+      <c r="V126" s="19"/>
+      <c r="W126" s="19"/>
+      <c r="X126" s="19"/>
+      <c r="Y126" s="19"/>
+      <c r="Z126" s="19"/>
+      <c r="AA126" s="19"/>
       <c r="AC126">
         <f>18-4.5</f>
         <v>13.5</v>
@@ -6827,13 +6820,6 @@
         <v>5.1585000000000001</v>
       </c>
       <c r="T170"/>
-      <c r="U170"/>
-      <c r="V170"/>
-      <c r="W170"/>
-      <c r="X170"/>
-      <c r="Y170"/>
-      <c r="Z170"/>
-      <c r="AA170"/>
     </row>
     <row r="171" spans="1:45" x14ac:dyDescent="0.3">
       <c r="G171" t="s">
@@ -6906,13 +6892,6 @@
       </c>
       <c r="R172" s="14"/>
       <c r="T172"/>
-      <c r="U172"/>
-      <c r="V172"/>
-      <c r="W172"/>
-      <c r="X172"/>
-      <c r="Y172"/>
-      <c r="Z172"/>
-      <c r="AA172"/>
     </row>
     <row r="173" spans="1:45" x14ac:dyDescent="0.3">
       <c r="H173" t="s">
@@ -6937,13 +6916,6 @@
         <v>18.452000000000002</v>
       </c>
       <c r="T173"/>
-      <c r="U173"/>
-      <c r="V173"/>
-      <c r="W173"/>
-      <c r="X173"/>
-      <c r="Y173"/>
-      <c r="Z173"/>
-      <c r="AA173"/>
     </row>
     <row r="174" spans="1:45" x14ac:dyDescent="0.3">
       <c r="G174" t="s">
@@ -6971,13 +6943,6 @@
         <v>10.5</v>
       </c>
       <c r="T174"/>
-      <c r="U174"/>
-      <c r="V174"/>
-      <c r="W174"/>
-      <c r="X174"/>
-      <c r="Y174"/>
-      <c r="Z174"/>
-      <c r="AA174"/>
     </row>
     <row r="175" spans="1:45" x14ac:dyDescent="0.3">
       <c r="H175" t="s">
@@ -7002,13 +6967,6 @@
         <v>16.5</v>
       </c>
       <c r="T175"/>
-      <c r="U175"/>
-      <c r="V175"/>
-      <c r="W175"/>
-      <c r="X175"/>
-      <c r="Y175"/>
-      <c r="Z175"/>
-      <c r="AA175"/>
     </row>
     <row r="176" spans="1:45" x14ac:dyDescent="0.3">
       <c r="H176" t="s">
@@ -7033,13 +6991,6 @@
         <v>2.6381999999999999</v>
       </c>
       <c r="T176"/>
-      <c r="U176"/>
-      <c r="V176"/>
-      <c r="W176"/>
-      <c r="X176"/>
-      <c r="Y176"/>
-      <c r="Z176"/>
-      <c r="AA176"/>
     </row>
     <row r="177" spans="1:35" x14ac:dyDescent="0.3">
       <c r="G177" t="s">
@@ -7067,13 +7018,6 @@
         <v>17</v>
       </c>
       <c r="T177"/>
-      <c r="U177"/>
-      <c r="V177"/>
-      <c r="W177"/>
-      <c r="X177"/>
-      <c r="Y177"/>
-      <c r="Z177"/>
-      <c r="AA177"/>
       <c r="AI177" s="14"/>
     </row>
     <row r="178" spans="1:35" x14ac:dyDescent="0.3">
@@ -7099,13 +7043,6 @@
         <v>19.5</v>
       </c>
       <c r="T178"/>
-      <c r="U178"/>
-      <c r="V178"/>
-      <c r="W178"/>
-      <c r="X178"/>
-      <c r="Y178"/>
-      <c r="Z178"/>
-      <c r="AA178"/>
       <c r="AI178" s="14"/>
     </row>
     <row r="179" spans="1:35" x14ac:dyDescent="0.3">
@@ -7192,13 +7129,6 @@
       </c>
       <c r="S181" s="14"/>
       <c r="T181"/>
-      <c r="U181"/>
-      <c r="V181"/>
-      <c r="W181"/>
-      <c r="X181"/>
-      <c r="Y181"/>
-      <c r="Z181"/>
-      <c r="AA181"/>
       <c r="AI181" s="14"/>
     </row>
     <row r="182" spans="1:35" x14ac:dyDescent="0.3">
@@ -7226,13 +7156,6 @@
       </c>
       <c r="S182" s="14"/>
       <c r="T182"/>
-      <c r="U182"/>
-      <c r="V182"/>
-      <c r="W182"/>
-      <c r="X182"/>
-      <c r="Y182"/>
-      <c r="Z182"/>
-      <c r="AA182"/>
       <c r="AH182" s="14"/>
       <c r="AI182" s="14"/>
     </row>
@@ -7263,13 +7186,6 @@
       </c>
       <c r="S183" s="14"/>
       <c r="T183"/>
-      <c r="U183"/>
-      <c r="V183"/>
-      <c r="W183"/>
-      <c r="X183"/>
-      <c r="Y183"/>
-      <c r="Z183"/>
-      <c r="AA183"/>
     </row>
     <row r="184" spans="1:35" x14ac:dyDescent="0.3">
       <c r="G184" s="14"/>
@@ -7296,13 +7212,6 @@
       </c>
       <c r="S184" s="14"/>
       <c r="T184"/>
-      <c r="U184"/>
-      <c r="V184"/>
-      <c r="W184"/>
-      <c r="X184"/>
-      <c r="Y184"/>
-      <c r="Z184"/>
-      <c r="AA184"/>
       <c r="AI184" s="14"/>
     </row>
     <row r="185" spans="1:35" x14ac:dyDescent="0.3">
@@ -7329,16 +7238,12 @@
         <v>20</v>
       </c>
       <c r="T185"/>
-      <c r="U185"/>
-      <c r="V185"/>
-      <c r="W185"/>
-      <c r="X185"/>
-      <c r="Y185"/>
-      <c r="Z185"/>
-      <c r="AA185"/>
       <c r="AI185" s="14"/>
     </row>
     <row r="186" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="F186">
+        <v>15</v>
+      </c>
       <c r="G186" t="s">
         <v>3</v>
       </c>
@@ -7375,13 +7280,6 @@
     <row r="187" spans="1:35" x14ac:dyDescent="0.3">
       <c r="S187" s="14"/>
       <c r="T187"/>
-      <c r="U187"/>
-      <c r="V187"/>
-      <c r="W187"/>
-      <c r="X187"/>
-      <c r="Y187"/>
-      <c r="Z187"/>
-      <c r="AA187"/>
       <c r="AF187" s="14"/>
       <c r="AG187" s="14"/>
       <c r="AI187" s="14"/>
@@ -7389,69 +7287,27 @@
     <row r="188" spans="1:35" x14ac:dyDescent="0.3">
       <c r="S188" s="14"/>
       <c r="T188"/>
-      <c r="U188"/>
-      <c r="V188"/>
-      <c r="W188"/>
-      <c r="X188"/>
-      <c r="Y188"/>
-      <c r="Z188"/>
-      <c r="AA188"/>
       <c r="AI188" s="14"/>
     </row>
     <row r="189" spans="1:35" x14ac:dyDescent="0.3">
       <c r="S189" s="14"/>
       <c r="T189"/>
-      <c r="U189"/>
-      <c r="V189"/>
-      <c r="W189"/>
-      <c r="X189"/>
-      <c r="Y189"/>
-      <c r="Z189"/>
-      <c r="AA189"/>
       <c r="AI189" s="14"/>
     </row>
     <row r="190" spans="1:35" x14ac:dyDescent="0.3">
       <c r="T190"/>
-      <c r="U190"/>
-      <c r="V190"/>
-      <c r="W190"/>
-      <c r="X190"/>
-      <c r="Y190"/>
-      <c r="Z190"/>
-      <c r="AA190"/>
       <c r="AI190" s="14"/>
     </row>
     <row r="191" spans="1:35" x14ac:dyDescent="0.3">
       <c r="T191"/>
-      <c r="U191"/>
-      <c r="V191"/>
-      <c r="W191"/>
-      <c r="X191"/>
-      <c r="Y191"/>
-      <c r="Z191"/>
-      <c r="AA191"/>
     </row>
     <row r="192" spans="1:35" x14ac:dyDescent="0.3">
       <c r="S192" s="14"/>
       <c r="T192"/>
-      <c r="U192"/>
-      <c r="V192"/>
-      <c r="W192"/>
-      <c r="X192"/>
-      <c r="Y192"/>
-      <c r="Z192"/>
-      <c r="AA192"/>
     </row>
     <row r="193" spans="19:33" x14ac:dyDescent="0.3">
       <c r="S193" s="14"/>
       <c r="T193"/>
-      <c r="U193"/>
-      <c r="V193"/>
-      <c r="W193"/>
-      <c r="X193"/>
-      <c r="Y193"/>
-      <c r="Z193"/>
-      <c r="AA193"/>
     </row>
     <row r="194" spans="19:33" x14ac:dyDescent="0.3">
       <c r="S194" s="14"/>
@@ -7462,85 +7318,29 @@
     </row>
     <row r="195" spans="19:33" x14ac:dyDescent="0.3">
       <c r="T195"/>
-      <c r="U195"/>
-      <c r="V195"/>
-      <c r="W195"/>
-      <c r="X195"/>
-      <c r="Y195"/>
-      <c r="Z195"/>
-      <c r="AA195"/>
     </row>
     <row r="196" spans="19:33" x14ac:dyDescent="0.3">
       <c r="T196"/>
-      <c r="U196"/>
-      <c r="V196"/>
-      <c r="W196"/>
-      <c r="X196"/>
-      <c r="Y196"/>
-      <c r="Z196"/>
-      <c r="AA196"/>
     </row>
     <row r="197" spans="19:33" x14ac:dyDescent="0.3">
       <c r="T197"/>
-      <c r="U197"/>
-      <c r="V197"/>
-      <c r="W197"/>
-      <c r="X197"/>
-      <c r="Y197"/>
-      <c r="Z197"/>
-      <c r="AA197"/>
     </row>
     <row r="198" spans="19:33" x14ac:dyDescent="0.3">
       <c r="T198"/>
-      <c r="U198"/>
-      <c r="V198"/>
-      <c r="W198"/>
-      <c r="X198"/>
-      <c r="Y198"/>
-      <c r="Z198"/>
-      <c r="AA198"/>
     </row>
     <row r="199" spans="19:33" x14ac:dyDescent="0.3">
       <c r="T199"/>
-      <c r="U199"/>
-      <c r="V199"/>
-      <c r="W199"/>
-      <c r="X199"/>
-      <c r="Y199"/>
-      <c r="Z199"/>
-      <c r="AA199"/>
     </row>
     <row r="200" spans="19:33" x14ac:dyDescent="0.3">
       <c r="T200"/>
-      <c r="U200"/>
-      <c r="V200"/>
-      <c r="W200"/>
-      <c r="X200"/>
-      <c r="Y200"/>
-      <c r="Z200"/>
-      <c r="AA200"/>
       <c r="AD200" s="14"/>
     </row>
     <row r="201" spans="19:33" x14ac:dyDescent="0.3">
       <c r="T201"/>
-      <c r="U201"/>
-      <c r="V201"/>
-      <c r="W201"/>
-      <c r="X201"/>
-      <c r="Y201"/>
-      <c r="Z201"/>
-      <c r="AA201"/>
       <c r="AD201" s="14"/>
     </row>
     <row r="202" spans="19:33" x14ac:dyDescent="0.3">
       <c r="T202"/>
-      <c r="U202"/>
-      <c r="V202"/>
-      <c r="W202"/>
-      <c r="X202"/>
-      <c r="Y202"/>
-      <c r="Z202"/>
-      <c r="AA202"/>
     </row>
     <row r="203" spans="19:33" x14ac:dyDescent="0.3">
       <c r="U203" s="14"/>
@@ -7559,63 +7359,21 @@
     </row>
     <row r="204" spans="19:33" x14ac:dyDescent="0.3">
       <c r="T204"/>
-      <c r="U204"/>
-      <c r="V204"/>
-      <c r="W204"/>
-      <c r="X204"/>
-      <c r="Y204"/>
-      <c r="Z204"/>
-      <c r="AA204"/>
     </row>
     <row r="205" spans="19:33" x14ac:dyDescent="0.3">
       <c r="T205"/>
-      <c r="U205"/>
-      <c r="V205"/>
-      <c r="W205"/>
-      <c r="X205"/>
-      <c r="Y205"/>
-      <c r="Z205"/>
-      <c r="AA205"/>
     </row>
     <row r="206" spans="19:33" x14ac:dyDescent="0.3">
       <c r="T206"/>
-      <c r="U206"/>
-      <c r="V206"/>
-      <c r="W206"/>
-      <c r="X206"/>
-      <c r="Y206"/>
-      <c r="Z206"/>
-      <c r="AA206"/>
     </row>
     <row r="207" spans="19:33" x14ac:dyDescent="0.3">
       <c r="T207"/>
-      <c r="U207"/>
-      <c r="V207"/>
-      <c r="W207"/>
-      <c r="X207"/>
-      <c r="Y207"/>
-      <c r="Z207"/>
-      <c r="AA207"/>
     </row>
     <row r="208" spans="19:33" x14ac:dyDescent="0.3">
       <c r="T208"/>
-      <c r="U208"/>
-      <c r="V208"/>
-      <c r="W208"/>
-      <c r="X208"/>
-      <c r="Y208"/>
-      <c r="Z208"/>
-      <c r="AA208"/>
-    </row>
-    <row r="209" spans="20:27" x14ac:dyDescent="0.3">
+    </row>
+    <row r="209" spans="20:20" x14ac:dyDescent="0.3">
       <c r="T209"/>
-      <c r="U209"/>
-      <c r="V209"/>
-      <c r="W209"/>
-      <c r="X209"/>
-      <c r="Y209"/>
-      <c r="Z209"/>
-      <c r="AA209"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
updated for new cs scattering results and to include as-run data frame controler
</commit_message>
<xml_diff>
--- a/cal/cal_results/CS_Ilena_Scattering_Results.xlsx
+++ b/cal/cal_results/CS_Ilena_Scattering_Results.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonny Woof\Google Drive\Python_packages_woof\pyMAP\cal\cal_results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31E6E24A-DA59-4F80-90B4-943C087A439A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1137102-FD2E-47EB-BBA8-CFE82E540FD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-11550" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cutfit fwhm" sheetId="3" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="72">
   <si>
     <t>100A</t>
   </si>
@@ -223,6 +224,33 @@
   </si>
   <si>
     <t>None</t>
+  </si>
+  <si>
+    <t>&gt; 21</t>
+  </si>
+  <si>
+    <t>FM-061</t>
+  </si>
+  <si>
+    <t>FM-093</t>
+  </si>
+  <si>
+    <t>FM-110</t>
+  </si>
+  <si>
+    <t>EM-036</t>
+  </si>
+  <si>
+    <t>EM-039</t>
+  </si>
+  <si>
+    <t>039b</t>
+  </si>
+  <si>
+    <t>Note</t>
+  </si>
+  <si>
+    <t>I believe the only difference between EM-039 and 039b is that one gives the total recoil ion efficiency  including sputtering and the other not including sputtering</t>
   </si>
 </sst>
 </file>
@@ -894,10 +922,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:AS209"/>
+  <dimension ref="A2:AS246"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A169" zoomScale="77" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F186" sqref="F186"/>
+    <sheetView tabSelected="1" topLeftCell="A129" zoomScale="77" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F155" sqref="F155"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6734,8 +6762,8 @@
       <c r="A168" t="s">
         <v>41</v>
       </c>
-      <c r="B168">
-        <v>39</v>
+      <c r="B168" t="s">
+        <v>69</v>
       </c>
       <c r="C168" t="s">
         <v>56</v>
@@ -7278,6 +7306,39 @@
       <c r="AI186" s="14"/>
     </row>
     <row r="187" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A187" t="s">
+        <v>41</v>
+      </c>
+      <c r="B187" t="s">
+        <v>64</v>
+      </c>
+      <c r="F187">
+        <v>8</v>
+      </c>
+      <c r="G187" t="s">
+        <v>3</v>
+      </c>
+      <c r="H187" t="s">
+        <v>59</v>
+      </c>
+      <c r="I187">
+        <v>1.7</v>
+      </c>
+      <c r="J187">
+        <v>1.7</v>
+      </c>
+      <c r="K187">
+        <v>1.3</v>
+      </c>
+      <c r="L187">
+        <v>1.4</v>
+      </c>
+      <c r="M187">
+        <v>1.9</v>
+      </c>
+      <c r="N187">
+        <v>2.1</v>
+      </c>
       <c r="S187" s="14"/>
       <c r="T187"/>
       <c r="AF187" s="14"/>
@@ -7285,95 +7346,1715 @@
       <c r="AI187" s="14"/>
     </row>
     <row r="188" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="S188" s="14"/>
-      <c r="T188"/>
-      <c r="AI188" s="14"/>
+      <c r="B188" t="s">
+        <v>64</v>
+      </c>
+      <c r="G188" t="s">
+        <v>3</v>
+      </c>
+      <c r="H188" t="s">
+        <v>33</v>
+      </c>
+      <c r="I188">
+        <v>13.7</v>
+      </c>
+      <c r="J188">
+        <v>14.2</v>
+      </c>
+      <c r="K188">
+        <v>15</v>
+      </c>
+      <c r="L188">
+        <v>14.6</v>
+      </c>
+      <c r="M188">
+        <v>14</v>
+      </c>
+      <c r="N188">
+        <v>13.8</v>
+      </c>
     </row>
     <row r="189" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="S189" s="14"/>
-      <c r="T189"/>
-      <c r="AI189" s="14"/>
+      <c r="B189" t="s">
+        <v>64</v>
+      </c>
+      <c r="G189" t="s">
+        <v>3</v>
+      </c>
+      <c r="H189" t="s">
+        <v>32</v>
+      </c>
+      <c r="I189">
+        <v>18.7</v>
+      </c>
+      <c r="J189">
+        <v>19.600000000000001</v>
+      </c>
+      <c r="K189">
+        <v>20</v>
+      </c>
+      <c r="L189" t="s">
+        <v>63</v>
+      </c>
+      <c r="M189" t="s">
+        <v>63</v>
+      </c>
+      <c r="N189" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="190" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="T190"/>
-      <c r="AI190" s="14"/>
+      <c r="B190" t="s">
+        <v>64</v>
+      </c>
+      <c r="G190" t="s">
+        <v>4</v>
+      </c>
+      <c r="H190" t="s">
+        <v>59</v>
+      </c>
+      <c r="I190">
+        <v>1.5</v>
+      </c>
+      <c r="J190">
+        <v>1.7</v>
+      </c>
+      <c r="K190">
+        <v>2</v>
+      </c>
+      <c r="L190">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="M190">
+        <v>2.7</v>
+      </c>
+      <c r="N190">
+        <v>2.2999999999999998</v>
+      </c>
     </row>
     <row r="191" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="T191"/>
+      <c r="B191" t="s">
+        <v>64</v>
+      </c>
+      <c r="G191" t="s">
+        <v>4</v>
+      </c>
+      <c r="H191" t="s">
+        <v>33</v>
+      </c>
+      <c r="I191">
+        <v>12.7</v>
+      </c>
+      <c r="J191">
+        <v>11.8</v>
+      </c>
+      <c r="K191">
+        <v>11.2</v>
+      </c>
+      <c r="L191">
+        <v>12</v>
+      </c>
+      <c r="M191">
+        <v>12.5</v>
+      </c>
+      <c r="N191">
+        <v>13</v>
+      </c>
     </row>
     <row r="192" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="S192" s="14"/>
-      <c r="T192"/>
-    </row>
-    <row r="193" spans="19:33" x14ac:dyDescent="0.3">
-      <c r="S193" s="14"/>
-      <c r="T193"/>
-    </row>
-    <row r="194" spans="19:33" x14ac:dyDescent="0.3">
-      <c r="S194" s="14"/>
-      <c r="AC194" s="14"/>
-      <c r="AD194" s="14"/>
-      <c r="AE194" s="14"/>
-      <c r="AF194" s="14"/>
-    </row>
-    <row r="195" spans="19:33" x14ac:dyDescent="0.3">
-      <c r="T195"/>
-    </row>
-    <row r="196" spans="19:33" x14ac:dyDescent="0.3">
-      <c r="T196"/>
-    </row>
-    <row r="197" spans="19:33" x14ac:dyDescent="0.3">
-      <c r="T197"/>
-    </row>
-    <row r="198" spans="19:33" x14ac:dyDescent="0.3">
-      <c r="T198"/>
-    </row>
-    <row r="199" spans="19:33" x14ac:dyDescent="0.3">
-      <c r="T199"/>
-    </row>
-    <row r="200" spans="19:33" x14ac:dyDescent="0.3">
-      <c r="T200"/>
-      <c r="AD200" s="14"/>
-    </row>
-    <row r="201" spans="19:33" x14ac:dyDescent="0.3">
-      <c r="T201"/>
-      <c r="AD201" s="14"/>
-    </row>
-    <row r="202" spans="19:33" x14ac:dyDescent="0.3">
-      <c r="T202"/>
-    </row>
-    <row r="203" spans="19:33" x14ac:dyDescent="0.3">
-      <c r="U203" s="14"/>
-      <c r="V203" s="14"/>
-      <c r="W203" s="14"/>
-      <c r="X203" s="14"/>
-      <c r="Y203" s="14"/>
-      <c r="Z203" s="14"/>
-      <c r="AA203" s="14"/>
-      <c r="AB203" s="14"/>
-      <c r="AC203" s="14"/>
-      <c r="AD203" s="14"/>
-      <c r="AE203" s="14"/>
-      <c r="AF203" s="14"/>
-      <c r="AG203" s="14"/>
-    </row>
-    <row r="204" spans="19:33" x14ac:dyDescent="0.3">
-      <c r="T204"/>
-    </row>
-    <row r="205" spans="19:33" x14ac:dyDescent="0.3">
-      <c r="T205"/>
-    </row>
-    <row r="206" spans="19:33" x14ac:dyDescent="0.3">
-      <c r="T206"/>
-    </row>
-    <row r="207" spans="19:33" x14ac:dyDescent="0.3">
-      <c r="T207"/>
-    </row>
-    <row r="208" spans="19:33" x14ac:dyDescent="0.3">
-      <c r="T208"/>
-    </row>
-    <row r="209" spans="20:20" x14ac:dyDescent="0.3">
-      <c r="T209"/>
+      <c r="B192" t="s">
+        <v>64</v>
+      </c>
+      <c r="G192" t="s">
+        <v>4</v>
+      </c>
+      <c r="H192" t="s">
+        <v>32</v>
+      </c>
+      <c r="I192">
+        <v>16.5</v>
+      </c>
+      <c r="J192">
+        <v>16.5</v>
+      </c>
+      <c r="K192">
+        <v>16.600000000000001</v>
+      </c>
+      <c r="L192">
+        <v>17.8</v>
+      </c>
+      <c r="M192">
+        <v>19.2</v>
+      </c>
+      <c r="N192">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="193" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B193" t="s">
+        <v>64</v>
+      </c>
+      <c r="G193" t="s">
+        <v>6</v>
+      </c>
+      <c r="H193" t="s">
+        <v>59</v>
+      </c>
+      <c r="I193" t="s">
+        <v>9</v>
+      </c>
+      <c r="J193">
+        <v>3.5</v>
+      </c>
+      <c r="K193">
+        <v>4</v>
+      </c>
+      <c r="L193">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="M193">
+        <v>4.2</v>
+      </c>
+      <c r="N193">
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="194" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B194" t="s">
+        <v>64</v>
+      </c>
+      <c r="G194" t="s">
+        <v>6</v>
+      </c>
+      <c r="H194" t="s">
+        <v>33</v>
+      </c>
+      <c r="I194" t="s">
+        <v>9</v>
+      </c>
+      <c r="J194">
+        <v>12.9</v>
+      </c>
+      <c r="K194">
+        <v>12.6</v>
+      </c>
+      <c r="L194">
+        <v>13</v>
+      </c>
+      <c r="M194">
+        <v>13.2</v>
+      </c>
+      <c r="N194">
+        <v>13.4</v>
+      </c>
+    </row>
+    <row r="195" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B195" t="s">
+        <v>64</v>
+      </c>
+      <c r="G195" t="s">
+        <v>6</v>
+      </c>
+      <c r="H195" t="s">
+        <v>32</v>
+      </c>
+      <c r="I195" t="s">
+        <v>9</v>
+      </c>
+      <c r="J195">
+        <v>15.5</v>
+      </c>
+      <c r="K195">
+        <v>15.8</v>
+      </c>
+      <c r="L195">
+        <v>16.3</v>
+      </c>
+      <c r="M195">
+        <v>17.399999999999999</v>
+      </c>
+      <c r="N195">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="196" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B196" t="s">
+        <v>64</v>
+      </c>
+      <c r="G196" t="s">
+        <v>5</v>
+      </c>
+      <c r="H196" t="s">
+        <v>59</v>
+      </c>
+      <c r="I196">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="J196">
+        <v>9.6</v>
+      </c>
+      <c r="K196">
+        <v>10.8</v>
+      </c>
+      <c r="L196">
+        <v>11.4</v>
+      </c>
+      <c r="M196">
+        <v>12.9</v>
+      </c>
+      <c r="N196">
+        <v>13.3</v>
+      </c>
+    </row>
+    <row r="197" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B197" t="s">
+        <v>64</v>
+      </c>
+      <c r="G197" t="s">
+        <v>5</v>
+      </c>
+      <c r="H197" t="s">
+        <v>33</v>
+      </c>
+      <c r="I197">
+        <v>10.3</v>
+      </c>
+      <c r="J197">
+        <v>10.8</v>
+      </c>
+      <c r="K197">
+        <v>11.6</v>
+      </c>
+      <c r="L197">
+        <v>13</v>
+      </c>
+      <c r="M197">
+        <v>15.3</v>
+      </c>
+      <c r="N197">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="198" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B198" t="s">
+        <v>64</v>
+      </c>
+      <c r="G198" t="s">
+        <v>5</v>
+      </c>
+      <c r="H198" t="s">
+        <v>32</v>
+      </c>
+      <c r="I198">
+        <v>14.4</v>
+      </c>
+      <c r="J198">
+        <v>15.3</v>
+      </c>
+      <c r="K198">
+        <v>16</v>
+      </c>
+      <c r="L198">
+        <v>17.399999999999999</v>
+      </c>
+      <c r="M198">
+        <v>20</v>
+      </c>
+      <c r="N198" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="199" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B199" t="s">
+        <v>65</v>
+      </c>
+      <c r="G199" t="s">
+        <v>3</v>
+      </c>
+      <c r="H199" t="s">
+        <v>59</v>
+      </c>
+      <c r="I199" t="s">
+        <v>9</v>
+      </c>
+      <c r="J199" t="s">
+        <v>9</v>
+      </c>
+      <c r="K199">
+        <v>1.9</v>
+      </c>
+      <c r="L199">
+        <v>1.6</v>
+      </c>
+      <c r="M199">
+        <v>1.9</v>
+      </c>
+      <c r="N199">
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="200" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B200" t="s">
+        <v>65</v>
+      </c>
+      <c r="G200" t="s">
+        <v>3</v>
+      </c>
+      <c r="H200" t="s">
+        <v>33</v>
+      </c>
+      <c r="I200" t="s">
+        <v>9</v>
+      </c>
+      <c r="J200" t="s">
+        <v>9</v>
+      </c>
+      <c r="K200">
+        <v>17</v>
+      </c>
+      <c r="L200">
+        <v>13.7</v>
+      </c>
+      <c r="M200">
+        <v>13</v>
+      </c>
+      <c r="N200">
+        <v>13.4</v>
+      </c>
+    </row>
+    <row r="201" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B201" t="s">
+        <v>65</v>
+      </c>
+      <c r="G201" t="s">
+        <v>3</v>
+      </c>
+      <c r="H201" t="s">
+        <v>32</v>
+      </c>
+      <c r="I201" t="s">
+        <v>9</v>
+      </c>
+      <c r="J201" t="s">
+        <v>9</v>
+      </c>
+      <c r="K201" t="s">
+        <v>9</v>
+      </c>
+      <c r="L201" t="s">
+        <v>9</v>
+      </c>
+      <c r="M201" t="s">
+        <v>9</v>
+      </c>
+      <c r="N201" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="202" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B202" t="s">
+        <v>65</v>
+      </c>
+      <c r="G202" t="s">
+        <v>4</v>
+      </c>
+      <c r="H202" t="s">
+        <v>59</v>
+      </c>
+      <c r="I202" t="s">
+        <v>9</v>
+      </c>
+      <c r="J202" t="s">
+        <v>9</v>
+      </c>
+      <c r="K202">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="L202">
+        <v>2.4</v>
+      </c>
+      <c r="M202">
+        <v>2.7</v>
+      </c>
+      <c r="N202">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="203" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B203" t="s">
+        <v>65</v>
+      </c>
+      <c r="G203" t="s">
+        <v>4</v>
+      </c>
+      <c r="H203" t="s">
+        <v>33</v>
+      </c>
+      <c r="I203" t="s">
+        <v>9</v>
+      </c>
+      <c r="J203" t="s">
+        <v>9</v>
+      </c>
+      <c r="K203">
+        <v>10.8</v>
+      </c>
+      <c r="L203">
+        <v>11.1</v>
+      </c>
+      <c r="M203">
+        <v>14.5</v>
+      </c>
+      <c r="N203">
+        <v>12.6</v>
+      </c>
+    </row>
+    <row r="204" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B204" t="s">
+        <v>65</v>
+      </c>
+      <c r="G204" t="s">
+        <v>4</v>
+      </c>
+      <c r="H204" t="s">
+        <v>32</v>
+      </c>
+      <c r="I204" t="s">
+        <v>9</v>
+      </c>
+      <c r="J204" t="s">
+        <v>9</v>
+      </c>
+      <c r="K204">
+        <v>15</v>
+      </c>
+      <c r="L204">
+        <v>15.5</v>
+      </c>
+      <c r="M204">
+        <v>21</v>
+      </c>
+      <c r="N204">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="205" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B205" t="s">
+        <v>65</v>
+      </c>
+      <c r="G205" t="s">
+        <v>6</v>
+      </c>
+      <c r="H205" t="s">
+        <v>59</v>
+      </c>
+      <c r="I205" t="s">
+        <v>9</v>
+      </c>
+      <c r="J205" t="s">
+        <v>9</v>
+      </c>
+      <c r="K205">
+        <v>3.7</v>
+      </c>
+      <c r="L205">
+        <v>3.8</v>
+      </c>
+      <c r="M205">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="N205">
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="206" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B206" t="s">
+        <v>65</v>
+      </c>
+      <c r="G206" t="s">
+        <v>6</v>
+      </c>
+      <c r="H206" t="s">
+        <v>33</v>
+      </c>
+      <c r="I206" t="s">
+        <v>9</v>
+      </c>
+      <c r="J206" t="s">
+        <v>9</v>
+      </c>
+      <c r="K206">
+        <v>10.8</v>
+      </c>
+      <c r="L206">
+        <v>11.1</v>
+      </c>
+      <c r="M206">
+        <v>11.5</v>
+      </c>
+      <c r="N206">
+        <v>12.2</v>
+      </c>
+    </row>
+    <row r="207" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B207" t="s">
+        <v>65</v>
+      </c>
+      <c r="G207" t="s">
+        <v>6</v>
+      </c>
+      <c r="H207" t="s">
+        <v>32</v>
+      </c>
+      <c r="I207" t="s">
+        <v>9</v>
+      </c>
+      <c r="J207" t="s">
+        <v>9</v>
+      </c>
+      <c r="K207">
+        <v>14.4</v>
+      </c>
+      <c r="L207">
+        <v>15</v>
+      </c>
+      <c r="M207">
+        <v>15.5</v>
+      </c>
+      <c r="N207">
+        <v>16.8</v>
+      </c>
+    </row>
+    <row r="208" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B208" t="s">
+        <v>65</v>
+      </c>
+      <c r="G208" t="s">
+        <v>5</v>
+      </c>
+      <c r="H208" t="s">
+        <v>59</v>
+      </c>
+      <c r="I208" t="s">
+        <v>9</v>
+      </c>
+      <c r="J208" t="s">
+        <v>9</v>
+      </c>
+      <c r="K208">
+        <v>10.3</v>
+      </c>
+      <c r="L208">
+        <v>11.6</v>
+      </c>
+      <c r="M208">
+        <v>12.3</v>
+      </c>
+      <c r="N208">
+        <v>12.6</v>
+      </c>
+    </row>
+    <row r="209" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B209" t="s">
+        <v>65</v>
+      </c>
+      <c r="G209" t="s">
+        <v>5</v>
+      </c>
+      <c r="H209" t="s">
+        <v>33</v>
+      </c>
+      <c r="I209" t="s">
+        <v>9</v>
+      </c>
+      <c r="J209" t="s">
+        <v>9</v>
+      </c>
+      <c r="K209">
+        <v>11</v>
+      </c>
+      <c r="L209">
+        <v>12.7</v>
+      </c>
+      <c r="M209">
+        <v>13.5</v>
+      </c>
+      <c r="N209">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="210" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B210" t="s">
+        <v>65</v>
+      </c>
+      <c r="G210" t="s">
+        <v>5</v>
+      </c>
+      <c r="H210" t="s">
+        <v>32</v>
+      </c>
+      <c r="I210" t="s">
+        <v>9</v>
+      </c>
+      <c r="J210" t="s">
+        <v>9</v>
+      </c>
+      <c r="K210">
+        <v>15</v>
+      </c>
+      <c r="L210">
+        <v>16.2</v>
+      </c>
+      <c r="M210">
+        <v>18</v>
+      </c>
+      <c r="N210">
+        <v>19.2</v>
+      </c>
+    </row>
+    <row r="211" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B211" t="s">
+        <v>66</v>
+      </c>
+      <c r="G211" t="s">
+        <v>3</v>
+      </c>
+      <c r="H211" t="s">
+        <v>59</v>
+      </c>
+      <c r="I211" t="s">
+        <v>9</v>
+      </c>
+      <c r="J211" t="s">
+        <v>9</v>
+      </c>
+      <c r="K211">
+        <v>1.3</v>
+      </c>
+      <c r="L211">
+        <v>1.8</v>
+      </c>
+      <c r="M211">
+        <v>1.5</v>
+      </c>
+      <c r="N211">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="212" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B212" t="s">
+        <v>66</v>
+      </c>
+      <c r="G212" t="s">
+        <v>3</v>
+      </c>
+      <c r="H212" t="s">
+        <v>33</v>
+      </c>
+      <c r="I212" t="s">
+        <v>9</v>
+      </c>
+      <c r="J212" t="s">
+        <v>9</v>
+      </c>
+      <c r="K212">
+        <v>15.3</v>
+      </c>
+      <c r="L212">
+        <v>15</v>
+      </c>
+      <c r="M212">
+        <v>14.3</v>
+      </c>
+      <c r="N212">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="213" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B213" t="s">
+        <v>66</v>
+      </c>
+      <c r="G213" t="s">
+        <v>3</v>
+      </c>
+      <c r="H213" t="s">
+        <v>32</v>
+      </c>
+      <c r="I213" t="s">
+        <v>9</v>
+      </c>
+      <c r="J213" t="s">
+        <v>9</v>
+      </c>
+      <c r="K213">
+        <v>19.5</v>
+      </c>
+      <c r="L213">
+        <v>21</v>
+      </c>
+      <c r="M213" t="s">
+        <v>63</v>
+      </c>
+      <c r="N213" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="214" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B214" t="s">
+        <v>66</v>
+      </c>
+      <c r="G214" t="s">
+        <v>4</v>
+      </c>
+      <c r="H214" t="s">
+        <v>59</v>
+      </c>
+      <c r="I214" t="s">
+        <v>9</v>
+      </c>
+      <c r="J214" t="s">
+        <v>9</v>
+      </c>
+      <c r="K214">
+        <v>2.85</v>
+      </c>
+      <c r="L214">
+        <v>2.4500000000000002</v>
+      </c>
+      <c r="M214">
+        <v>2.9</v>
+      </c>
+      <c r="N214">
+        <v>3.2</v>
+      </c>
+    </row>
+    <row r="215" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B215" t="s">
+        <v>66</v>
+      </c>
+      <c r="G215" t="s">
+        <v>4</v>
+      </c>
+      <c r="H215" t="s">
+        <v>33</v>
+      </c>
+      <c r="I215" t="s">
+        <v>9</v>
+      </c>
+      <c r="J215" t="s">
+        <v>9</v>
+      </c>
+      <c r="K215">
+        <v>12.2</v>
+      </c>
+      <c r="L215">
+        <v>12.7</v>
+      </c>
+      <c r="M215">
+        <v>17.8</v>
+      </c>
+      <c r="N215">
+        <v>15.5</v>
+      </c>
+    </row>
+    <row r="216" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B216" t="s">
+        <v>66</v>
+      </c>
+      <c r="G216" t="s">
+        <v>4</v>
+      </c>
+      <c r="H216" t="s">
+        <v>32</v>
+      </c>
+      <c r="I216" t="s">
+        <v>9</v>
+      </c>
+      <c r="J216" t="s">
+        <v>9</v>
+      </c>
+      <c r="K216">
+        <v>17.2</v>
+      </c>
+      <c r="L216">
+        <v>19</v>
+      </c>
+      <c r="M216">
+        <v>21</v>
+      </c>
+      <c r="N216" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="217" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B217" t="s">
+        <v>66</v>
+      </c>
+      <c r="G217" t="s">
+        <v>6</v>
+      </c>
+      <c r="H217" t="s">
+        <v>59</v>
+      </c>
+      <c r="I217" t="s">
+        <v>9</v>
+      </c>
+      <c r="J217" t="s">
+        <v>9</v>
+      </c>
+      <c r="K217">
+        <v>4.2</v>
+      </c>
+      <c r="L217">
+        <v>4.3</v>
+      </c>
+      <c r="M217">
+        <v>4</v>
+      </c>
+      <c r="N217">
+        <v>4.7</v>
+      </c>
+    </row>
+    <row r="218" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B218" t="s">
+        <v>66</v>
+      </c>
+      <c r="G218" t="s">
+        <v>6</v>
+      </c>
+      <c r="H218" t="s">
+        <v>33</v>
+      </c>
+      <c r="I218" t="s">
+        <v>9</v>
+      </c>
+      <c r="J218" t="s">
+        <v>9</v>
+      </c>
+      <c r="K218">
+        <v>13.1</v>
+      </c>
+      <c r="L218">
+        <v>13</v>
+      </c>
+      <c r="M218">
+        <v>13.6</v>
+      </c>
+      <c r="N218">
+        <v>14.1</v>
+      </c>
+    </row>
+    <row r="219" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B219" t="s">
+        <v>66</v>
+      </c>
+      <c r="G219" t="s">
+        <v>6</v>
+      </c>
+      <c r="H219" t="s">
+        <v>32</v>
+      </c>
+      <c r="I219" t="s">
+        <v>9</v>
+      </c>
+      <c r="J219" t="s">
+        <v>9</v>
+      </c>
+      <c r="K219">
+        <v>15.8</v>
+      </c>
+      <c r="L219">
+        <v>16</v>
+      </c>
+      <c r="M219">
+        <v>16.7</v>
+      </c>
+      <c r="N219">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="220" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B220" t="s">
+        <v>66</v>
+      </c>
+      <c r="G220" t="s">
+        <v>5</v>
+      </c>
+      <c r="H220" t="s">
+        <v>59</v>
+      </c>
+      <c r="I220" t="s">
+        <v>9</v>
+      </c>
+      <c r="J220" t="s">
+        <v>9</v>
+      </c>
+      <c r="K220">
+        <v>11.3</v>
+      </c>
+      <c r="L220">
+        <v>12.8</v>
+      </c>
+      <c r="M220">
+        <v>14.2</v>
+      </c>
+      <c r="N220">
+        <v>13.9</v>
+      </c>
+    </row>
+    <row r="221" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B221" t="s">
+        <v>66</v>
+      </c>
+      <c r="G221" t="s">
+        <v>5</v>
+      </c>
+      <c r="H221" t="s">
+        <v>33</v>
+      </c>
+      <c r="I221" t="s">
+        <v>9</v>
+      </c>
+      <c r="J221" t="s">
+        <v>9</v>
+      </c>
+      <c r="K221">
+        <v>12.3</v>
+      </c>
+      <c r="L221">
+        <v>13</v>
+      </c>
+      <c r="M221">
+        <v>15</v>
+      </c>
+      <c r="N221">
+        <v>16.2</v>
+      </c>
+    </row>
+    <row r="222" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B222" t="s">
+        <v>66</v>
+      </c>
+      <c r="G222" t="s">
+        <v>5</v>
+      </c>
+      <c r="H222" t="s">
+        <v>32</v>
+      </c>
+      <c r="I222" t="s">
+        <v>9</v>
+      </c>
+      <c r="J222" t="s">
+        <v>9</v>
+      </c>
+      <c r="K222">
+        <v>15.6</v>
+      </c>
+      <c r="L222">
+        <v>15.9</v>
+      </c>
+      <c r="M222">
+        <v>19</v>
+      </c>
+      <c r="N222" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="223" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B223" t="s">
+        <v>67</v>
+      </c>
+      <c r="G223" t="s">
+        <v>3</v>
+      </c>
+      <c r="H223" t="s">
+        <v>59</v>
+      </c>
+      <c r="I223">
+        <v>1.7</v>
+      </c>
+      <c r="J223">
+        <v>1.7</v>
+      </c>
+      <c r="K223">
+        <v>1.3</v>
+      </c>
+      <c r="L223">
+        <v>1.4</v>
+      </c>
+      <c r="M223">
+        <v>1.9</v>
+      </c>
+      <c r="N223">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="224" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B224" t="s">
+        <v>67</v>
+      </c>
+      <c r="G224" t="s">
+        <v>3</v>
+      </c>
+      <c r="H224" t="s">
+        <v>33</v>
+      </c>
+      <c r="I224">
+        <v>14.5</v>
+      </c>
+      <c r="J224">
+        <v>16.8</v>
+      </c>
+      <c r="K224">
+        <v>15.7</v>
+      </c>
+      <c r="L224">
+        <v>15</v>
+      </c>
+      <c r="M224">
+        <v>14.7</v>
+      </c>
+      <c r="N224">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="225" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B225" t="s">
+        <v>67</v>
+      </c>
+      <c r="G225" t="s">
+        <v>3</v>
+      </c>
+      <c r="H225" t="s">
+        <v>32</v>
+      </c>
+      <c r="I225">
+        <v>19.5</v>
+      </c>
+      <c r="J225">
+        <v>21</v>
+      </c>
+      <c r="K225">
+        <v>21.7</v>
+      </c>
+      <c r="L225">
+        <v>22</v>
+      </c>
+      <c r="M225">
+        <v>22.7</v>
+      </c>
+      <c r="N225">
+        <v>23.3</v>
+      </c>
+    </row>
+    <row r="226" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B226" t="s">
+        <v>67</v>
+      </c>
+      <c r="G226" t="s">
+        <v>4</v>
+      </c>
+      <c r="H226" t="s">
+        <v>59</v>
+      </c>
+      <c r="I226">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="J226">
+        <v>2.5</v>
+      </c>
+      <c r="K226">
+        <v>2.9</v>
+      </c>
+      <c r="L226">
+        <v>3</v>
+      </c>
+      <c r="M226">
+        <v>3</v>
+      </c>
+      <c r="N226">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="227" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B227" t="s">
+        <v>67</v>
+      </c>
+      <c r="G227" t="s">
+        <v>4</v>
+      </c>
+      <c r="H227" t="s">
+        <v>33</v>
+      </c>
+      <c r="I227">
+        <v>14</v>
+      </c>
+      <c r="J227">
+        <v>13.7</v>
+      </c>
+      <c r="K227">
+        <v>12.5</v>
+      </c>
+      <c r="L227">
+        <v>12.8</v>
+      </c>
+      <c r="M227">
+        <v>13.4</v>
+      </c>
+      <c r="N227">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="228" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B228" t="s">
+        <v>67</v>
+      </c>
+      <c r="G228" t="s">
+        <v>4</v>
+      </c>
+      <c r="H228" t="s">
+        <v>32</v>
+      </c>
+      <c r="I228">
+        <v>18</v>
+      </c>
+      <c r="J228">
+        <v>17</v>
+      </c>
+      <c r="K228">
+        <v>16.5</v>
+      </c>
+      <c r="L228">
+        <v>18.5</v>
+      </c>
+      <c r="M228">
+        <v>20</v>
+      </c>
+      <c r="N228">
+        <v>21.5</v>
+      </c>
+    </row>
+    <row r="229" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B229" t="s">
+        <v>67</v>
+      </c>
+      <c r="G229" t="s">
+        <v>6</v>
+      </c>
+      <c r="H229" t="s">
+        <v>59</v>
+      </c>
+      <c r="I229">
+        <v>3.5</v>
+      </c>
+      <c r="J229">
+        <v>3.6</v>
+      </c>
+      <c r="K229">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="L229">
+        <v>4.3</v>
+      </c>
+      <c r="M229">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="N229">
+        <v>4.9000000000000004</v>
+      </c>
+    </row>
+    <row r="230" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B230" t="s">
+        <v>67</v>
+      </c>
+      <c r="G230" t="s">
+        <v>6</v>
+      </c>
+      <c r="H230" t="s">
+        <v>33</v>
+      </c>
+      <c r="I230">
+        <v>12</v>
+      </c>
+      <c r="J230">
+        <v>13</v>
+      </c>
+      <c r="K230">
+        <v>12.7</v>
+      </c>
+      <c r="L230">
+        <v>12.4</v>
+      </c>
+      <c r="M230">
+        <v>13.5</v>
+      </c>
+      <c r="N230">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="231" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B231" t="s">
+        <v>67</v>
+      </c>
+      <c r="G231" t="s">
+        <v>6</v>
+      </c>
+      <c r="H231" t="s">
+        <v>32</v>
+      </c>
+      <c r="I231">
+        <v>15.5</v>
+      </c>
+      <c r="J231">
+        <v>16</v>
+      </c>
+      <c r="K231">
+        <v>15.5</v>
+      </c>
+      <c r="L231">
+        <v>15.5</v>
+      </c>
+      <c r="M231">
+        <v>16.5</v>
+      </c>
+      <c r="N231">
+        <v>19.5</v>
+      </c>
+    </row>
+    <row r="232" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B232" t="s">
+        <v>67</v>
+      </c>
+      <c r="G232" t="s">
+        <v>5</v>
+      </c>
+      <c r="H232" t="s">
+        <v>59</v>
+      </c>
+      <c r="I232">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="J232">
+        <v>9.4</v>
+      </c>
+      <c r="K232">
+        <v>11</v>
+      </c>
+      <c r="L232">
+        <v>11.9</v>
+      </c>
+      <c r="M232">
+        <v>12.4</v>
+      </c>
+      <c r="N232">
+        <v>12.4</v>
+      </c>
+    </row>
+    <row r="233" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B233" t="s">
+        <v>67</v>
+      </c>
+      <c r="G233" t="s">
+        <v>5</v>
+      </c>
+      <c r="H233" t="s">
+        <v>33</v>
+      </c>
+      <c r="I233">
+        <v>10.6</v>
+      </c>
+      <c r="J233">
+        <v>10.4</v>
+      </c>
+      <c r="K233">
+        <v>13</v>
+      </c>
+      <c r="L233">
+        <v>13.5</v>
+      </c>
+      <c r="M233">
+        <v>14.7</v>
+      </c>
+      <c r="N233">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="234" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B234" t="s">
+        <v>67</v>
+      </c>
+      <c r="G234" t="s">
+        <v>5</v>
+      </c>
+      <c r="H234" t="s">
+        <v>32</v>
+      </c>
+      <c r="I234">
+        <v>14.2</v>
+      </c>
+      <c r="J234">
+        <v>14</v>
+      </c>
+      <c r="K234">
+        <v>14.8</v>
+      </c>
+      <c r="L234">
+        <v>16.5</v>
+      </c>
+      <c r="M234">
+        <v>19.5</v>
+      </c>
+      <c r="N234">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="235" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B235" t="s">
+        <v>68</v>
+      </c>
+      <c r="G235" t="s">
+        <v>3</v>
+      </c>
+      <c r="H235" t="s">
+        <v>59</v>
+      </c>
+      <c r="I235">
+        <v>1.9</v>
+      </c>
+      <c r="J235">
+        <v>1.8</v>
+      </c>
+      <c r="K235">
+        <v>1.5</v>
+      </c>
+      <c r="L235">
+        <v>1.6</v>
+      </c>
+      <c r="M235">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="N235">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="236" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B236" t="s">
+        <v>68</v>
+      </c>
+      <c r="G236" t="s">
+        <v>3</v>
+      </c>
+      <c r="H236" t="s">
+        <v>33</v>
+      </c>
+      <c r="I236">
+        <v>11.5</v>
+      </c>
+      <c r="J236">
+        <v>11.7</v>
+      </c>
+      <c r="K236">
+        <v>16</v>
+      </c>
+      <c r="L236">
+        <v>14.3</v>
+      </c>
+      <c r="M236">
+        <v>15.5</v>
+      </c>
+      <c r="N236">
+        <v>15.6</v>
+      </c>
+    </row>
+    <row r="237" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B237" t="s">
+        <v>68</v>
+      </c>
+      <c r="G237" t="s">
+        <v>3</v>
+      </c>
+      <c r="H237" t="s">
+        <v>32</v>
+      </c>
+      <c r="I237">
+        <v>15</v>
+      </c>
+      <c r="J237">
+        <v>14.5</v>
+      </c>
+      <c r="K237">
+        <v>21.5</v>
+      </c>
+      <c r="L237">
+        <v>21.8</v>
+      </c>
+      <c r="M237">
+        <v>22</v>
+      </c>
+      <c r="N237">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="238" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B238" t="s">
+        <v>68</v>
+      </c>
+      <c r="G238" t="s">
+        <v>4</v>
+      </c>
+      <c r="H238" t="s">
+        <v>59</v>
+      </c>
+      <c r="I238">
+        <v>1.6</v>
+      </c>
+      <c r="J238">
+        <v>2</v>
+      </c>
+      <c r="K238">
+        <v>2.5</v>
+      </c>
+      <c r="L238">
+        <v>2.6</v>
+      </c>
+      <c r="M238">
+        <v>2.6</v>
+      </c>
+      <c r="N238">
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="239" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B239" t="s">
+        <v>68</v>
+      </c>
+      <c r="G239" t="s">
+        <v>4</v>
+      </c>
+      <c r="H239" t="s">
+        <v>33</v>
+      </c>
+      <c r="I239">
+        <v>11.3</v>
+      </c>
+      <c r="J239">
+        <v>10.3</v>
+      </c>
+      <c r="K239">
+        <v>10.5</v>
+      </c>
+      <c r="L239">
+        <v>9.5</v>
+      </c>
+      <c r="M239">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="N239">
+        <v>10.5</v>
+      </c>
+    </row>
+    <row r="240" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B240" t="s">
+        <v>68</v>
+      </c>
+      <c r="G240" t="s">
+        <v>4</v>
+      </c>
+      <c r="H240" t="s">
+        <v>32</v>
+      </c>
+      <c r="I240">
+        <v>14.5</v>
+      </c>
+      <c r="J240">
+        <v>13.5</v>
+      </c>
+      <c r="K240">
+        <v>14</v>
+      </c>
+      <c r="L240">
+        <v>13.7</v>
+      </c>
+      <c r="M240">
+        <v>14.3</v>
+      </c>
+      <c r="N240">
+        <v>16.5</v>
+      </c>
+    </row>
+    <row r="241" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B241" t="s">
+        <v>68</v>
+      </c>
+      <c r="G241" t="s">
+        <v>6</v>
+      </c>
+      <c r="H241" t="s">
+        <v>59</v>
+      </c>
+      <c r="I241">
+        <v>2.9</v>
+      </c>
+      <c r="J241">
+        <v>2.8</v>
+      </c>
+      <c r="K241">
+        <v>3.5</v>
+      </c>
+      <c r="L241">
+        <v>3.6</v>
+      </c>
+      <c r="M241">
+        <v>4</v>
+      </c>
+      <c r="N241">
+        <v>3.7</v>
+      </c>
+    </row>
+    <row r="242" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B242" t="s">
+        <v>68</v>
+      </c>
+      <c r="G242" t="s">
+        <v>6</v>
+      </c>
+      <c r="H242" t="s">
+        <v>33</v>
+      </c>
+      <c r="I242">
+        <v>11.7</v>
+      </c>
+      <c r="J242">
+        <v>11</v>
+      </c>
+      <c r="K242">
+        <v>10</v>
+      </c>
+      <c r="L242">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="M242">
+        <v>10.3</v>
+      </c>
+      <c r="N242">
+        <v>10.4</v>
+      </c>
+    </row>
+    <row r="243" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B243" t="s">
+        <v>68</v>
+      </c>
+      <c r="G243" t="s">
+        <v>6</v>
+      </c>
+      <c r="H243" t="s">
+        <v>32</v>
+      </c>
+      <c r="I243">
+        <v>14.5</v>
+      </c>
+      <c r="J243">
+        <v>13.8</v>
+      </c>
+      <c r="K243">
+        <v>12.5</v>
+      </c>
+      <c r="L243">
+        <v>12.5</v>
+      </c>
+      <c r="M243">
+        <v>13.5</v>
+      </c>
+      <c r="N243">
+        <v>13.5</v>
+      </c>
+    </row>
+    <row r="244" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B244" t="s">
+        <v>68</v>
+      </c>
+      <c r="G244" t="s">
+        <v>5</v>
+      </c>
+      <c r="H244" t="s">
+        <v>59</v>
+      </c>
+      <c r="I244">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="J244">
+        <v>10</v>
+      </c>
+      <c r="K244">
+        <v>11.9</v>
+      </c>
+      <c r="L244">
+        <v>12.8</v>
+      </c>
+      <c r="M244">
+        <v>14</v>
+      </c>
+      <c r="N244">
+        <v>14.8</v>
+      </c>
+    </row>
+    <row r="245" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B245" t="s">
+        <v>68</v>
+      </c>
+      <c r="G245" t="s">
+        <v>5</v>
+      </c>
+      <c r="H245" t="s">
+        <v>33</v>
+      </c>
+      <c r="I245">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="J245">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="K245">
+        <v>8.9</v>
+      </c>
+      <c r="L245">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="M245">
+        <v>13.4</v>
+      </c>
+      <c r="N245">
+        <v>13.9</v>
+      </c>
+    </row>
+    <row r="246" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B246" t="s">
+        <v>68</v>
+      </c>
+      <c r="G246" t="s">
+        <v>5</v>
+      </c>
+      <c r="H246" t="s">
+        <v>32</v>
+      </c>
+      <c r="I246">
+        <v>12</v>
+      </c>
+      <c r="J246">
+        <v>12.5</v>
+      </c>
+      <c r="K246">
+        <v>12.2</v>
+      </c>
+      <c r="L246">
+        <v>13.5</v>
+      </c>
+      <c r="M246">
+        <v>17.3</v>
+      </c>
+      <c r="N246">
+        <v>18.2</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -7387,4 +9068,27 @@
     <ignoredError sqref="P48 R106" formula="1"/>
   </ignoredErrors>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47E15288-D17F-4056-8745-CA72DD924B6E}">
+  <dimension ref="A3:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="R9" sqref="R9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>